<commit_message>
closes issue#1, closes issue #9
I think I've worked out the bugs with selecting the right collection
member from multiple possible matches. I also added some simple logic to
deal with handling a shelf location if one exists.
</commit_message>
<xml_diff>
--- a/Macro File/daily rtf test.xlsx
+++ b/Macro File/daily rtf test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service Center\Documents\GitHub\RTFprototypes\Macro File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blake\Documents\GitHub\RTFprototypes\Macro File\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Daily RTF report" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1679,7 +1680,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2016,653 +2017,655 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" customWidth="1"/>
-    <col min="6" max="6" width="41.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" customWidth="1"/>
-    <col min="8" max="8" width="4.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="29" customWidth="1"/>
-    <col min="257" max="257" width="14.81640625" customWidth="1"/>
+    <col min="257" max="257" width="14.85546875" customWidth="1"/>
     <col min="258" max="258" width="12" customWidth="1"/>
-    <col min="259" max="259" width="18.54296875" customWidth="1"/>
-    <col min="260" max="260" width="20.54296875" customWidth="1"/>
-    <col min="261" max="261" width="9.54296875" customWidth="1"/>
-    <col min="262" max="262" width="41.1796875" customWidth="1"/>
-    <col min="263" max="263" width="13.7265625" customWidth="1"/>
-    <col min="264" max="264" width="4.81640625" customWidth="1"/>
+    <col min="259" max="259" width="18.5703125" customWidth="1"/>
+    <col min="260" max="260" width="20.5703125" customWidth="1"/>
+    <col min="261" max="261" width="9.5703125" customWidth="1"/>
+    <col min="262" max="262" width="41.140625" customWidth="1"/>
+    <col min="263" max="263" width="13.7109375" customWidth="1"/>
+    <col min="264" max="264" width="4.85546875" customWidth="1"/>
     <col min="265" max="265" width="0" hidden="1" customWidth="1"/>
     <col min="266" max="266" width="29" customWidth="1"/>
-    <col min="513" max="513" width="14.81640625" customWidth="1"/>
+    <col min="513" max="513" width="14.85546875" customWidth="1"/>
     <col min="514" max="514" width="12" customWidth="1"/>
-    <col min="515" max="515" width="18.54296875" customWidth="1"/>
-    <col min="516" max="516" width="20.54296875" customWidth="1"/>
-    <col min="517" max="517" width="9.54296875" customWidth="1"/>
-    <col min="518" max="518" width="41.1796875" customWidth="1"/>
-    <col min="519" max="519" width="13.7265625" customWidth="1"/>
-    <col min="520" max="520" width="4.81640625" customWidth="1"/>
+    <col min="515" max="515" width="18.5703125" customWidth="1"/>
+    <col min="516" max="516" width="20.5703125" customWidth="1"/>
+    <col min="517" max="517" width="9.5703125" customWidth="1"/>
+    <col min="518" max="518" width="41.140625" customWidth="1"/>
+    <col min="519" max="519" width="13.7109375" customWidth="1"/>
+    <col min="520" max="520" width="4.85546875" customWidth="1"/>
     <col min="521" max="521" width="0" hidden="1" customWidth="1"/>
     <col min="522" max="522" width="29" customWidth="1"/>
-    <col min="769" max="769" width="14.81640625" customWidth="1"/>
+    <col min="769" max="769" width="14.85546875" customWidth="1"/>
     <col min="770" max="770" width="12" customWidth="1"/>
-    <col min="771" max="771" width="18.54296875" customWidth="1"/>
-    <col min="772" max="772" width="20.54296875" customWidth="1"/>
-    <col min="773" max="773" width="9.54296875" customWidth="1"/>
-    <col min="774" max="774" width="41.1796875" customWidth="1"/>
-    <col min="775" max="775" width="13.7265625" customWidth="1"/>
-    <col min="776" max="776" width="4.81640625" customWidth="1"/>
+    <col min="771" max="771" width="18.5703125" customWidth="1"/>
+    <col min="772" max="772" width="20.5703125" customWidth="1"/>
+    <col min="773" max="773" width="9.5703125" customWidth="1"/>
+    <col min="774" max="774" width="41.140625" customWidth="1"/>
+    <col min="775" max="775" width="13.7109375" customWidth="1"/>
+    <col min="776" max="776" width="4.85546875" customWidth="1"/>
     <col min="777" max="777" width="0" hidden="1" customWidth="1"/>
     <col min="778" max="778" width="29" customWidth="1"/>
-    <col min="1025" max="1025" width="14.81640625" customWidth="1"/>
+    <col min="1025" max="1025" width="14.85546875" customWidth="1"/>
     <col min="1026" max="1026" width="12" customWidth="1"/>
-    <col min="1027" max="1027" width="18.54296875" customWidth="1"/>
-    <col min="1028" max="1028" width="20.54296875" customWidth="1"/>
-    <col min="1029" max="1029" width="9.54296875" customWidth="1"/>
-    <col min="1030" max="1030" width="41.1796875" customWidth="1"/>
-    <col min="1031" max="1031" width="13.7265625" customWidth="1"/>
-    <col min="1032" max="1032" width="4.81640625" customWidth="1"/>
+    <col min="1027" max="1027" width="18.5703125" customWidth="1"/>
+    <col min="1028" max="1028" width="20.5703125" customWidth="1"/>
+    <col min="1029" max="1029" width="9.5703125" customWidth="1"/>
+    <col min="1030" max="1030" width="41.140625" customWidth="1"/>
+    <col min="1031" max="1031" width="13.7109375" customWidth="1"/>
+    <col min="1032" max="1032" width="4.85546875" customWidth="1"/>
     <col min="1033" max="1033" width="0" hidden="1" customWidth="1"/>
     <col min="1034" max="1034" width="29" customWidth="1"/>
-    <col min="1281" max="1281" width="14.81640625" customWidth="1"/>
+    <col min="1281" max="1281" width="14.85546875" customWidth="1"/>
     <col min="1282" max="1282" width="12" customWidth="1"/>
-    <col min="1283" max="1283" width="18.54296875" customWidth="1"/>
-    <col min="1284" max="1284" width="20.54296875" customWidth="1"/>
-    <col min="1285" max="1285" width="9.54296875" customWidth="1"/>
-    <col min="1286" max="1286" width="41.1796875" customWidth="1"/>
-    <col min="1287" max="1287" width="13.7265625" customWidth="1"/>
-    <col min="1288" max="1288" width="4.81640625" customWidth="1"/>
+    <col min="1283" max="1283" width="18.5703125" customWidth="1"/>
+    <col min="1284" max="1284" width="20.5703125" customWidth="1"/>
+    <col min="1285" max="1285" width="9.5703125" customWidth="1"/>
+    <col min="1286" max="1286" width="41.140625" customWidth="1"/>
+    <col min="1287" max="1287" width="13.7109375" customWidth="1"/>
+    <col min="1288" max="1288" width="4.85546875" customWidth="1"/>
     <col min="1289" max="1289" width="0" hidden="1" customWidth="1"/>
     <col min="1290" max="1290" width="29" customWidth="1"/>
-    <col min="1537" max="1537" width="14.81640625" customWidth="1"/>
+    <col min="1537" max="1537" width="14.85546875" customWidth="1"/>
     <col min="1538" max="1538" width="12" customWidth="1"/>
-    <col min="1539" max="1539" width="18.54296875" customWidth="1"/>
-    <col min="1540" max="1540" width="20.54296875" customWidth="1"/>
-    <col min="1541" max="1541" width="9.54296875" customWidth="1"/>
-    <col min="1542" max="1542" width="41.1796875" customWidth="1"/>
-    <col min="1543" max="1543" width="13.7265625" customWidth="1"/>
-    <col min="1544" max="1544" width="4.81640625" customWidth="1"/>
+    <col min="1539" max="1539" width="18.5703125" customWidth="1"/>
+    <col min="1540" max="1540" width="20.5703125" customWidth="1"/>
+    <col min="1541" max="1541" width="9.5703125" customWidth="1"/>
+    <col min="1542" max="1542" width="41.140625" customWidth="1"/>
+    <col min="1543" max="1543" width="13.7109375" customWidth="1"/>
+    <col min="1544" max="1544" width="4.85546875" customWidth="1"/>
     <col min="1545" max="1545" width="0" hidden="1" customWidth="1"/>
     <col min="1546" max="1546" width="29" customWidth="1"/>
-    <col min="1793" max="1793" width="14.81640625" customWidth="1"/>
+    <col min="1793" max="1793" width="14.85546875" customWidth="1"/>
     <col min="1794" max="1794" width="12" customWidth="1"/>
-    <col min="1795" max="1795" width="18.54296875" customWidth="1"/>
-    <col min="1796" max="1796" width="20.54296875" customWidth="1"/>
-    <col min="1797" max="1797" width="9.54296875" customWidth="1"/>
-    <col min="1798" max="1798" width="41.1796875" customWidth="1"/>
-    <col min="1799" max="1799" width="13.7265625" customWidth="1"/>
-    <col min="1800" max="1800" width="4.81640625" customWidth="1"/>
+    <col min="1795" max="1795" width="18.5703125" customWidth="1"/>
+    <col min="1796" max="1796" width="20.5703125" customWidth="1"/>
+    <col min="1797" max="1797" width="9.5703125" customWidth="1"/>
+    <col min="1798" max="1798" width="41.140625" customWidth="1"/>
+    <col min="1799" max="1799" width="13.7109375" customWidth="1"/>
+    <col min="1800" max="1800" width="4.85546875" customWidth="1"/>
     <col min="1801" max="1801" width="0" hidden="1" customWidth="1"/>
     <col min="1802" max="1802" width="29" customWidth="1"/>
-    <col min="2049" max="2049" width="14.81640625" customWidth="1"/>
+    <col min="2049" max="2049" width="14.85546875" customWidth="1"/>
     <col min="2050" max="2050" width="12" customWidth="1"/>
-    <col min="2051" max="2051" width="18.54296875" customWidth="1"/>
-    <col min="2052" max="2052" width="20.54296875" customWidth="1"/>
-    <col min="2053" max="2053" width="9.54296875" customWidth="1"/>
-    <col min="2054" max="2054" width="41.1796875" customWidth="1"/>
-    <col min="2055" max="2055" width="13.7265625" customWidth="1"/>
-    <col min="2056" max="2056" width="4.81640625" customWidth="1"/>
+    <col min="2051" max="2051" width="18.5703125" customWidth="1"/>
+    <col min="2052" max="2052" width="20.5703125" customWidth="1"/>
+    <col min="2053" max="2053" width="9.5703125" customWidth="1"/>
+    <col min="2054" max="2054" width="41.140625" customWidth="1"/>
+    <col min="2055" max="2055" width="13.7109375" customWidth="1"/>
+    <col min="2056" max="2056" width="4.85546875" customWidth="1"/>
     <col min="2057" max="2057" width="0" hidden="1" customWidth="1"/>
     <col min="2058" max="2058" width="29" customWidth="1"/>
-    <col min="2305" max="2305" width="14.81640625" customWidth="1"/>
+    <col min="2305" max="2305" width="14.85546875" customWidth="1"/>
     <col min="2306" max="2306" width="12" customWidth="1"/>
-    <col min="2307" max="2307" width="18.54296875" customWidth="1"/>
-    <col min="2308" max="2308" width="20.54296875" customWidth="1"/>
-    <col min="2309" max="2309" width="9.54296875" customWidth="1"/>
-    <col min="2310" max="2310" width="41.1796875" customWidth="1"/>
-    <col min="2311" max="2311" width="13.7265625" customWidth="1"/>
-    <col min="2312" max="2312" width="4.81640625" customWidth="1"/>
+    <col min="2307" max="2307" width="18.5703125" customWidth="1"/>
+    <col min="2308" max="2308" width="20.5703125" customWidth="1"/>
+    <col min="2309" max="2309" width="9.5703125" customWidth="1"/>
+    <col min="2310" max="2310" width="41.140625" customWidth="1"/>
+    <col min="2311" max="2311" width="13.7109375" customWidth="1"/>
+    <col min="2312" max="2312" width="4.85546875" customWidth="1"/>
     <col min="2313" max="2313" width="0" hidden="1" customWidth="1"/>
     <col min="2314" max="2314" width="29" customWidth="1"/>
-    <col min="2561" max="2561" width="14.81640625" customWidth="1"/>
+    <col min="2561" max="2561" width="14.85546875" customWidth="1"/>
     <col min="2562" max="2562" width="12" customWidth="1"/>
-    <col min="2563" max="2563" width="18.54296875" customWidth="1"/>
-    <col min="2564" max="2564" width="20.54296875" customWidth="1"/>
-    <col min="2565" max="2565" width="9.54296875" customWidth="1"/>
-    <col min="2566" max="2566" width="41.1796875" customWidth="1"/>
-    <col min="2567" max="2567" width="13.7265625" customWidth="1"/>
-    <col min="2568" max="2568" width="4.81640625" customWidth="1"/>
+    <col min="2563" max="2563" width="18.5703125" customWidth="1"/>
+    <col min="2564" max="2564" width="20.5703125" customWidth="1"/>
+    <col min="2565" max="2565" width="9.5703125" customWidth="1"/>
+    <col min="2566" max="2566" width="41.140625" customWidth="1"/>
+    <col min="2567" max="2567" width="13.7109375" customWidth="1"/>
+    <col min="2568" max="2568" width="4.85546875" customWidth="1"/>
     <col min="2569" max="2569" width="0" hidden="1" customWidth="1"/>
     <col min="2570" max="2570" width="29" customWidth="1"/>
-    <col min="2817" max="2817" width="14.81640625" customWidth="1"/>
+    <col min="2817" max="2817" width="14.85546875" customWidth="1"/>
     <col min="2818" max="2818" width="12" customWidth="1"/>
-    <col min="2819" max="2819" width="18.54296875" customWidth="1"/>
-    <col min="2820" max="2820" width="20.54296875" customWidth="1"/>
-    <col min="2821" max="2821" width="9.54296875" customWidth="1"/>
-    <col min="2822" max="2822" width="41.1796875" customWidth="1"/>
-    <col min="2823" max="2823" width="13.7265625" customWidth="1"/>
-    <col min="2824" max="2824" width="4.81640625" customWidth="1"/>
+    <col min="2819" max="2819" width="18.5703125" customWidth="1"/>
+    <col min="2820" max="2820" width="20.5703125" customWidth="1"/>
+    <col min="2821" max="2821" width="9.5703125" customWidth="1"/>
+    <col min="2822" max="2822" width="41.140625" customWidth="1"/>
+    <col min="2823" max="2823" width="13.7109375" customWidth="1"/>
+    <col min="2824" max="2824" width="4.85546875" customWidth="1"/>
     <col min="2825" max="2825" width="0" hidden="1" customWidth="1"/>
     <col min="2826" max="2826" width="29" customWidth="1"/>
-    <col min="3073" max="3073" width="14.81640625" customWidth="1"/>
+    <col min="3073" max="3073" width="14.85546875" customWidth="1"/>
     <col min="3074" max="3074" width="12" customWidth="1"/>
-    <col min="3075" max="3075" width="18.54296875" customWidth="1"/>
-    <col min="3076" max="3076" width="20.54296875" customWidth="1"/>
-    <col min="3077" max="3077" width="9.54296875" customWidth="1"/>
-    <col min="3078" max="3078" width="41.1796875" customWidth="1"/>
-    <col min="3079" max="3079" width="13.7265625" customWidth="1"/>
-    <col min="3080" max="3080" width="4.81640625" customWidth="1"/>
+    <col min="3075" max="3075" width="18.5703125" customWidth="1"/>
+    <col min="3076" max="3076" width="20.5703125" customWidth="1"/>
+    <col min="3077" max="3077" width="9.5703125" customWidth="1"/>
+    <col min="3078" max="3078" width="41.140625" customWidth="1"/>
+    <col min="3079" max="3079" width="13.7109375" customWidth="1"/>
+    <col min="3080" max="3080" width="4.85546875" customWidth="1"/>
     <col min="3081" max="3081" width="0" hidden="1" customWidth="1"/>
     <col min="3082" max="3082" width="29" customWidth="1"/>
-    <col min="3329" max="3329" width="14.81640625" customWidth="1"/>
+    <col min="3329" max="3329" width="14.85546875" customWidth="1"/>
     <col min="3330" max="3330" width="12" customWidth="1"/>
-    <col min="3331" max="3331" width="18.54296875" customWidth="1"/>
-    <col min="3332" max="3332" width="20.54296875" customWidth="1"/>
-    <col min="3333" max="3333" width="9.54296875" customWidth="1"/>
-    <col min="3334" max="3334" width="41.1796875" customWidth="1"/>
-    <col min="3335" max="3335" width="13.7265625" customWidth="1"/>
-    <col min="3336" max="3336" width="4.81640625" customWidth="1"/>
+    <col min="3331" max="3331" width="18.5703125" customWidth="1"/>
+    <col min="3332" max="3332" width="20.5703125" customWidth="1"/>
+    <col min="3333" max="3333" width="9.5703125" customWidth="1"/>
+    <col min="3334" max="3334" width="41.140625" customWidth="1"/>
+    <col min="3335" max="3335" width="13.7109375" customWidth="1"/>
+    <col min="3336" max="3336" width="4.85546875" customWidth="1"/>
     <col min="3337" max="3337" width="0" hidden="1" customWidth="1"/>
     <col min="3338" max="3338" width="29" customWidth="1"/>
-    <col min="3585" max="3585" width="14.81640625" customWidth="1"/>
+    <col min="3585" max="3585" width="14.85546875" customWidth="1"/>
     <col min="3586" max="3586" width="12" customWidth="1"/>
-    <col min="3587" max="3587" width="18.54296875" customWidth="1"/>
-    <col min="3588" max="3588" width="20.54296875" customWidth="1"/>
-    <col min="3589" max="3589" width="9.54296875" customWidth="1"/>
-    <col min="3590" max="3590" width="41.1796875" customWidth="1"/>
-    <col min="3591" max="3591" width="13.7265625" customWidth="1"/>
-    <col min="3592" max="3592" width="4.81640625" customWidth="1"/>
+    <col min="3587" max="3587" width="18.5703125" customWidth="1"/>
+    <col min="3588" max="3588" width="20.5703125" customWidth="1"/>
+    <col min="3589" max="3589" width="9.5703125" customWidth="1"/>
+    <col min="3590" max="3590" width="41.140625" customWidth="1"/>
+    <col min="3591" max="3591" width="13.7109375" customWidth="1"/>
+    <col min="3592" max="3592" width="4.85546875" customWidth="1"/>
     <col min="3593" max="3593" width="0" hidden="1" customWidth="1"/>
     <col min="3594" max="3594" width="29" customWidth="1"/>
-    <col min="3841" max="3841" width="14.81640625" customWidth="1"/>
+    <col min="3841" max="3841" width="14.85546875" customWidth="1"/>
     <col min="3842" max="3842" width="12" customWidth="1"/>
-    <col min="3843" max="3843" width="18.54296875" customWidth="1"/>
-    <col min="3844" max="3844" width="20.54296875" customWidth="1"/>
-    <col min="3845" max="3845" width="9.54296875" customWidth="1"/>
-    <col min="3846" max="3846" width="41.1796875" customWidth="1"/>
-    <col min="3847" max="3847" width="13.7265625" customWidth="1"/>
-    <col min="3848" max="3848" width="4.81640625" customWidth="1"/>
+    <col min="3843" max="3843" width="18.5703125" customWidth="1"/>
+    <col min="3844" max="3844" width="20.5703125" customWidth="1"/>
+    <col min="3845" max="3845" width="9.5703125" customWidth="1"/>
+    <col min="3846" max="3846" width="41.140625" customWidth="1"/>
+    <col min="3847" max="3847" width="13.7109375" customWidth="1"/>
+    <col min="3848" max="3848" width="4.85546875" customWidth="1"/>
     <col min="3849" max="3849" width="0" hidden="1" customWidth="1"/>
     <col min="3850" max="3850" width="29" customWidth="1"/>
-    <col min="4097" max="4097" width="14.81640625" customWidth="1"/>
+    <col min="4097" max="4097" width="14.85546875" customWidth="1"/>
     <col min="4098" max="4098" width="12" customWidth="1"/>
-    <col min="4099" max="4099" width="18.54296875" customWidth="1"/>
-    <col min="4100" max="4100" width="20.54296875" customWidth="1"/>
-    <col min="4101" max="4101" width="9.54296875" customWidth="1"/>
-    <col min="4102" max="4102" width="41.1796875" customWidth="1"/>
-    <col min="4103" max="4103" width="13.7265625" customWidth="1"/>
-    <col min="4104" max="4104" width="4.81640625" customWidth="1"/>
+    <col min="4099" max="4099" width="18.5703125" customWidth="1"/>
+    <col min="4100" max="4100" width="20.5703125" customWidth="1"/>
+    <col min="4101" max="4101" width="9.5703125" customWidth="1"/>
+    <col min="4102" max="4102" width="41.140625" customWidth="1"/>
+    <col min="4103" max="4103" width="13.7109375" customWidth="1"/>
+    <col min="4104" max="4104" width="4.85546875" customWidth="1"/>
     <col min="4105" max="4105" width="0" hidden="1" customWidth="1"/>
     <col min="4106" max="4106" width="29" customWidth="1"/>
-    <col min="4353" max="4353" width="14.81640625" customWidth="1"/>
+    <col min="4353" max="4353" width="14.85546875" customWidth="1"/>
     <col min="4354" max="4354" width="12" customWidth="1"/>
-    <col min="4355" max="4355" width="18.54296875" customWidth="1"/>
-    <col min="4356" max="4356" width="20.54296875" customWidth="1"/>
-    <col min="4357" max="4357" width="9.54296875" customWidth="1"/>
-    <col min="4358" max="4358" width="41.1796875" customWidth="1"/>
-    <col min="4359" max="4359" width="13.7265625" customWidth="1"/>
-    <col min="4360" max="4360" width="4.81640625" customWidth="1"/>
+    <col min="4355" max="4355" width="18.5703125" customWidth="1"/>
+    <col min="4356" max="4356" width="20.5703125" customWidth="1"/>
+    <col min="4357" max="4357" width="9.5703125" customWidth="1"/>
+    <col min="4358" max="4358" width="41.140625" customWidth="1"/>
+    <col min="4359" max="4359" width="13.7109375" customWidth="1"/>
+    <col min="4360" max="4360" width="4.85546875" customWidth="1"/>
     <col min="4361" max="4361" width="0" hidden="1" customWidth="1"/>
     <col min="4362" max="4362" width="29" customWidth="1"/>
-    <col min="4609" max="4609" width="14.81640625" customWidth="1"/>
+    <col min="4609" max="4609" width="14.85546875" customWidth="1"/>
     <col min="4610" max="4610" width="12" customWidth="1"/>
-    <col min="4611" max="4611" width="18.54296875" customWidth="1"/>
-    <col min="4612" max="4612" width="20.54296875" customWidth="1"/>
-    <col min="4613" max="4613" width="9.54296875" customWidth="1"/>
-    <col min="4614" max="4614" width="41.1796875" customWidth="1"/>
-    <col min="4615" max="4615" width="13.7265625" customWidth="1"/>
-    <col min="4616" max="4616" width="4.81640625" customWidth="1"/>
+    <col min="4611" max="4611" width="18.5703125" customWidth="1"/>
+    <col min="4612" max="4612" width="20.5703125" customWidth="1"/>
+    <col min="4613" max="4613" width="9.5703125" customWidth="1"/>
+    <col min="4614" max="4614" width="41.140625" customWidth="1"/>
+    <col min="4615" max="4615" width="13.7109375" customWidth="1"/>
+    <col min="4616" max="4616" width="4.85546875" customWidth="1"/>
     <col min="4617" max="4617" width="0" hidden="1" customWidth="1"/>
     <col min="4618" max="4618" width="29" customWidth="1"/>
-    <col min="4865" max="4865" width="14.81640625" customWidth="1"/>
+    <col min="4865" max="4865" width="14.85546875" customWidth="1"/>
     <col min="4866" max="4866" width="12" customWidth="1"/>
-    <col min="4867" max="4867" width="18.54296875" customWidth="1"/>
-    <col min="4868" max="4868" width="20.54296875" customWidth="1"/>
-    <col min="4869" max="4869" width="9.54296875" customWidth="1"/>
-    <col min="4870" max="4870" width="41.1796875" customWidth="1"/>
-    <col min="4871" max="4871" width="13.7265625" customWidth="1"/>
-    <col min="4872" max="4872" width="4.81640625" customWidth="1"/>
+    <col min="4867" max="4867" width="18.5703125" customWidth="1"/>
+    <col min="4868" max="4868" width="20.5703125" customWidth="1"/>
+    <col min="4869" max="4869" width="9.5703125" customWidth="1"/>
+    <col min="4870" max="4870" width="41.140625" customWidth="1"/>
+    <col min="4871" max="4871" width="13.7109375" customWidth="1"/>
+    <col min="4872" max="4872" width="4.85546875" customWidth="1"/>
     <col min="4873" max="4873" width="0" hidden="1" customWidth="1"/>
     <col min="4874" max="4874" width="29" customWidth="1"/>
-    <col min="5121" max="5121" width="14.81640625" customWidth="1"/>
+    <col min="5121" max="5121" width="14.85546875" customWidth="1"/>
     <col min="5122" max="5122" width="12" customWidth="1"/>
-    <col min="5123" max="5123" width="18.54296875" customWidth="1"/>
-    <col min="5124" max="5124" width="20.54296875" customWidth="1"/>
-    <col min="5125" max="5125" width="9.54296875" customWidth="1"/>
-    <col min="5126" max="5126" width="41.1796875" customWidth="1"/>
-    <col min="5127" max="5127" width="13.7265625" customWidth="1"/>
-    <col min="5128" max="5128" width="4.81640625" customWidth="1"/>
+    <col min="5123" max="5123" width="18.5703125" customWidth="1"/>
+    <col min="5124" max="5124" width="20.5703125" customWidth="1"/>
+    <col min="5125" max="5125" width="9.5703125" customWidth="1"/>
+    <col min="5126" max="5126" width="41.140625" customWidth="1"/>
+    <col min="5127" max="5127" width="13.7109375" customWidth="1"/>
+    <col min="5128" max="5128" width="4.85546875" customWidth="1"/>
     <col min="5129" max="5129" width="0" hidden="1" customWidth="1"/>
     <col min="5130" max="5130" width="29" customWidth="1"/>
-    <col min="5377" max="5377" width="14.81640625" customWidth="1"/>
+    <col min="5377" max="5377" width="14.85546875" customWidth="1"/>
     <col min="5378" max="5378" width="12" customWidth="1"/>
-    <col min="5379" max="5379" width="18.54296875" customWidth="1"/>
-    <col min="5380" max="5380" width="20.54296875" customWidth="1"/>
-    <col min="5381" max="5381" width="9.54296875" customWidth="1"/>
-    <col min="5382" max="5382" width="41.1796875" customWidth="1"/>
-    <col min="5383" max="5383" width="13.7265625" customWidth="1"/>
-    <col min="5384" max="5384" width="4.81640625" customWidth="1"/>
+    <col min="5379" max="5379" width="18.5703125" customWidth="1"/>
+    <col min="5380" max="5380" width="20.5703125" customWidth="1"/>
+    <col min="5381" max="5381" width="9.5703125" customWidth="1"/>
+    <col min="5382" max="5382" width="41.140625" customWidth="1"/>
+    <col min="5383" max="5383" width="13.7109375" customWidth="1"/>
+    <col min="5384" max="5384" width="4.85546875" customWidth="1"/>
     <col min="5385" max="5385" width="0" hidden="1" customWidth="1"/>
     <col min="5386" max="5386" width="29" customWidth="1"/>
-    <col min="5633" max="5633" width="14.81640625" customWidth="1"/>
+    <col min="5633" max="5633" width="14.85546875" customWidth="1"/>
     <col min="5634" max="5634" width="12" customWidth="1"/>
-    <col min="5635" max="5635" width="18.54296875" customWidth="1"/>
-    <col min="5636" max="5636" width="20.54296875" customWidth="1"/>
-    <col min="5637" max="5637" width="9.54296875" customWidth="1"/>
-    <col min="5638" max="5638" width="41.1796875" customWidth="1"/>
-    <col min="5639" max="5639" width="13.7265625" customWidth="1"/>
-    <col min="5640" max="5640" width="4.81640625" customWidth="1"/>
+    <col min="5635" max="5635" width="18.5703125" customWidth="1"/>
+    <col min="5636" max="5636" width="20.5703125" customWidth="1"/>
+    <col min="5637" max="5637" width="9.5703125" customWidth="1"/>
+    <col min="5638" max="5638" width="41.140625" customWidth="1"/>
+    <col min="5639" max="5639" width="13.7109375" customWidth="1"/>
+    <col min="5640" max="5640" width="4.85546875" customWidth="1"/>
     <col min="5641" max="5641" width="0" hidden="1" customWidth="1"/>
     <col min="5642" max="5642" width="29" customWidth="1"/>
-    <col min="5889" max="5889" width="14.81640625" customWidth="1"/>
+    <col min="5889" max="5889" width="14.85546875" customWidth="1"/>
     <col min="5890" max="5890" width="12" customWidth="1"/>
-    <col min="5891" max="5891" width="18.54296875" customWidth="1"/>
-    <col min="5892" max="5892" width="20.54296875" customWidth="1"/>
-    <col min="5893" max="5893" width="9.54296875" customWidth="1"/>
-    <col min="5894" max="5894" width="41.1796875" customWidth="1"/>
-    <col min="5895" max="5895" width="13.7265625" customWidth="1"/>
-    <col min="5896" max="5896" width="4.81640625" customWidth="1"/>
+    <col min="5891" max="5891" width="18.5703125" customWidth="1"/>
+    <col min="5892" max="5892" width="20.5703125" customWidth="1"/>
+    <col min="5893" max="5893" width="9.5703125" customWidth="1"/>
+    <col min="5894" max="5894" width="41.140625" customWidth="1"/>
+    <col min="5895" max="5895" width="13.7109375" customWidth="1"/>
+    <col min="5896" max="5896" width="4.85546875" customWidth="1"/>
     <col min="5897" max="5897" width="0" hidden="1" customWidth="1"/>
     <col min="5898" max="5898" width="29" customWidth="1"/>
-    <col min="6145" max="6145" width="14.81640625" customWidth="1"/>
+    <col min="6145" max="6145" width="14.85546875" customWidth="1"/>
     <col min="6146" max="6146" width="12" customWidth="1"/>
-    <col min="6147" max="6147" width="18.54296875" customWidth="1"/>
-    <col min="6148" max="6148" width="20.54296875" customWidth="1"/>
-    <col min="6149" max="6149" width="9.54296875" customWidth="1"/>
-    <col min="6150" max="6150" width="41.1796875" customWidth="1"/>
-    <col min="6151" max="6151" width="13.7265625" customWidth="1"/>
-    <col min="6152" max="6152" width="4.81640625" customWidth="1"/>
+    <col min="6147" max="6147" width="18.5703125" customWidth="1"/>
+    <col min="6148" max="6148" width="20.5703125" customWidth="1"/>
+    <col min="6149" max="6149" width="9.5703125" customWidth="1"/>
+    <col min="6150" max="6150" width="41.140625" customWidth="1"/>
+    <col min="6151" max="6151" width="13.7109375" customWidth="1"/>
+    <col min="6152" max="6152" width="4.85546875" customWidth="1"/>
     <col min="6153" max="6153" width="0" hidden="1" customWidth="1"/>
     <col min="6154" max="6154" width="29" customWidth="1"/>
-    <col min="6401" max="6401" width="14.81640625" customWidth="1"/>
+    <col min="6401" max="6401" width="14.85546875" customWidth="1"/>
     <col min="6402" max="6402" width="12" customWidth="1"/>
-    <col min="6403" max="6403" width="18.54296875" customWidth="1"/>
-    <col min="6404" max="6404" width="20.54296875" customWidth="1"/>
-    <col min="6405" max="6405" width="9.54296875" customWidth="1"/>
-    <col min="6406" max="6406" width="41.1796875" customWidth="1"/>
-    <col min="6407" max="6407" width="13.7265625" customWidth="1"/>
-    <col min="6408" max="6408" width="4.81640625" customWidth="1"/>
+    <col min="6403" max="6403" width="18.5703125" customWidth="1"/>
+    <col min="6404" max="6404" width="20.5703125" customWidth="1"/>
+    <col min="6405" max="6405" width="9.5703125" customWidth="1"/>
+    <col min="6406" max="6406" width="41.140625" customWidth="1"/>
+    <col min="6407" max="6407" width="13.7109375" customWidth="1"/>
+    <col min="6408" max="6408" width="4.85546875" customWidth="1"/>
     <col min="6409" max="6409" width="0" hidden="1" customWidth="1"/>
     <col min="6410" max="6410" width="29" customWidth="1"/>
-    <col min="6657" max="6657" width="14.81640625" customWidth="1"/>
+    <col min="6657" max="6657" width="14.85546875" customWidth="1"/>
     <col min="6658" max="6658" width="12" customWidth="1"/>
-    <col min="6659" max="6659" width="18.54296875" customWidth="1"/>
-    <col min="6660" max="6660" width="20.54296875" customWidth="1"/>
-    <col min="6661" max="6661" width="9.54296875" customWidth="1"/>
-    <col min="6662" max="6662" width="41.1796875" customWidth="1"/>
-    <col min="6663" max="6663" width="13.7265625" customWidth="1"/>
-    <col min="6664" max="6664" width="4.81640625" customWidth="1"/>
+    <col min="6659" max="6659" width="18.5703125" customWidth="1"/>
+    <col min="6660" max="6660" width="20.5703125" customWidth="1"/>
+    <col min="6661" max="6661" width="9.5703125" customWidth="1"/>
+    <col min="6662" max="6662" width="41.140625" customWidth="1"/>
+    <col min="6663" max="6663" width="13.7109375" customWidth="1"/>
+    <col min="6664" max="6664" width="4.85546875" customWidth="1"/>
     <col min="6665" max="6665" width="0" hidden="1" customWidth="1"/>
     <col min="6666" max="6666" width="29" customWidth="1"/>
-    <col min="6913" max="6913" width="14.81640625" customWidth="1"/>
+    <col min="6913" max="6913" width="14.85546875" customWidth="1"/>
     <col min="6914" max="6914" width="12" customWidth="1"/>
-    <col min="6915" max="6915" width="18.54296875" customWidth="1"/>
-    <col min="6916" max="6916" width="20.54296875" customWidth="1"/>
-    <col min="6917" max="6917" width="9.54296875" customWidth="1"/>
-    <col min="6918" max="6918" width="41.1796875" customWidth="1"/>
-    <col min="6919" max="6919" width="13.7265625" customWidth="1"/>
-    <col min="6920" max="6920" width="4.81640625" customWidth="1"/>
+    <col min="6915" max="6915" width="18.5703125" customWidth="1"/>
+    <col min="6916" max="6916" width="20.5703125" customWidth="1"/>
+    <col min="6917" max="6917" width="9.5703125" customWidth="1"/>
+    <col min="6918" max="6918" width="41.140625" customWidth="1"/>
+    <col min="6919" max="6919" width="13.7109375" customWidth="1"/>
+    <col min="6920" max="6920" width="4.85546875" customWidth="1"/>
     <col min="6921" max="6921" width="0" hidden="1" customWidth="1"/>
     <col min="6922" max="6922" width="29" customWidth="1"/>
-    <col min="7169" max="7169" width="14.81640625" customWidth="1"/>
+    <col min="7169" max="7169" width="14.85546875" customWidth="1"/>
     <col min="7170" max="7170" width="12" customWidth="1"/>
-    <col min="7171" max="7171" width="18.54296875" customWidth="1"/>
-    <col min="7172" max="7172" width="20.54296875" customWidth="1"/>
-    <col min="7173" max="7173" width="9.54296875" customWidth="1"/>
-    <col min="7174" max="7174" width="41.1796875" customWidth="1"/>
-    <col min="7175" max="7175" width="13.7265625" customWidth="1"/>
-    <col min="7176" max="7176" width="4.81640625" customWidth="1"/>
+    <col min="7171" max="7171" width="18.5703125" customWidth="1"/>
+    <col min="7172" max="7172" width="20.5703125" customWidth="1"/>
+    <col min="7173" max="7173" width="9.5703125" customWidth="1"/>
+    <col min="7174" max="7174" width="41.140625" customWidth="1"/>
+    <col min="7175" max="7175" width="13.7109375" customWidth="1"/>
+    <col min="7176" max="7176" width="4.85546875" customWidth="1"/>
     <col min="7177" max="7177" width="0" hidden="1" customWidth="1"/>
     <col min="7178" max="7178" width="29" customWidth="1"/>
-    <col min="7425" max="7425" width="14.81640625" customWidth="1"/>
+    <col min="7425" max="7425" width="14.85546875" customWidth="1"/>
     <col min="7426" max="7426" width="12" customWidth="1"/>
-    <col min="7427" max="7427" width="18.54296875" customWidth="1"/>
-    <col min="7428" max="7428" width="20.54296875" customWidth="1"/>
-    <col min="7429" max="7429" width="9.54296875" customWidth="1"/>
-    <col min="7430" max="7430" width="41.1796875" customWidth="1"/>
-    <col min="7431" max="7431" width="13.7265625" customWidth="1"/>
-    <col min="7432" max="7432" width="4.81640625" customWidth="1"/>
+    <col min="7427" max="7427" width="18.5703125" customWidth="1"/>
+    <col min="7428" max="7428" width="20.5703125" customWidth="1"/>
+    <col min="7429" max="7429" width="9.5703125" customWidth="1"/>
+    <col min="7430" max="7430" width="41.140625" customWidth="1"/>
+    <col min="7431" max="7431" width="13.7109375" customWidth="1"/>
+    <col min="7432" max="7432" width="4.85546875" customWidth="1"/>
     <col min="7433" max="7433" width="0" hidden="1" customWidth="1"/>
     <col min="7434" max="7434" width="29" customWidth="1"/>
-    <col min="7681" max="7681" width="14.81640625" customWidth="1"/>
+    <col min="7681" max="7681" width="14.85546875" customWidth="1"/>
     <col min="7682" max="7682" width="12" customWidth="1"/>
-    <col min="7683" max="7683" width="18.54296875" customWidth="1"/>
-    <col min="7684" max="7684" width="20.54296875" customWidth="1"/>
-    <col min="7685" max="7685" width="9.54296875" customWidth="1"/>
-    <col min="7686" max="7686" width="41.1796875" customWidth="1"/>
-    <col min="7687" max="7687" width="13.7265625" customWidth="1"/>
-    <col min="7688" max="7688" width="4.81640625" customWidth="1"/>
+    <col min="7683" max="7683" width="18.5703125" customWidth="1"/>
+    <col min="7684" max="7684" width="20.5703125" customWidth="1"/>
+    <col min="7685" max="7685" width="9.5703125" customWidth="1"/>
+    <col min="7686" max="7686" width="41.140625" customWidth="1"/>
+    <col min="7687" max="7687" width="13.7109375" customWidth="1"/>
+    <col min="7688" max="7688" width="4.85546875" customWidth="1"/>
     <col min="7689" max="7689" width="0" hidden="1" customWidth="1"/>
     <col min="7690" max="7690" width="29" customWidth="1"/>
-    <col min="7937" max="7937" width="14.81640625" customWidth="1"/>
+    <col min="7937" max="7937" width="14.85546875" customWidth="1"/>
     <col min="7938" max="7938" width="12" customWidth="1"/>
-    <col min="7939" max="7939" width="18.54296875" customWidth="1"/>
-    <col min="7940" max="7940" width="20.54296875" customWidth="1"/>
-    <col min="7941" max="7941" width="9.54296875" customWidth="1"/>
-    <col min="7942" max="7942" width="41.1796875" customWidth="1"/>
-    <col min="7943" max="7943" width="13.7265625" customWidth="1"/>
-    <col min="7944" max="7944" width="4.81640625" customWidth="1"/>
+    <col min="7939" max="7939" width="18.5703125" customWidth="1"/>
+    <col min="7940" max="7940" width="20.5703125" customWidth="1"/>
+    <col min="7941" max="7941" width="9.5703125" customWidth="1"/>
+    <col min="7942" max="7942" width="41.140625" customWidth="1"/>
+    <col min="7943" max="7943" width="13.7109375" customWidth="1"/>
+    <col min="7944" max="7944" width="4.85546875" customWidth="1"/>
     <col min="7945" max="7945" width="0" hidden="1" customWidth="1"/>
     <col min="7946" max="7946" width="29" customWidth="1"/>
-    <col min="8193" max="8193" width="14.81640625" customWidth="1"/>
+    <col min="8193" max="8193" width="14.85546875" customWidth="1"/>
     <col min="8194" max="8194" width="12" customWidth="1"/>
-    <col min="8195" max="8195" width="18.54296875" customWidth="1"/>
-    <col min="8196" max="8196" width="20.54296875" customWidth="1"/>
-    <col min="8197" max="8197" width="9.54296875" customWidth="1"/>
-    <col min="8198" max="8198" width="41.1796875" customWidth="1"/>
-    <col min="8199" max="8199" width="13.7265625" customWidth="1"/>
-    <col min="8200" max="8200" width="4.81640625" customWidth="1"/>
+    <col min="8195" max="8195" width="18.5703125" customWidth="1"/>
+    <col min="8196" max="8196" width="20.5703125" customWidth="1"/>
+    <col min="8197" max="8197" width="9.5703125" customWidth="1"/>
+    <col min="8198" max="8198" width="41.140625" customWidth="1"/>
+    <col min="8199" max="8199" width="13.7109375" customWidth="1"/>
+    <col min="8200" max="8200" width="4.85546875" customWidth="1"/>
     <col min="8201" max="8201" width="0" hidden="1" customWidth="1"/>
     <col min="8202" max="8202" width="29" customWidth="1"/>
-    <col min="8449" max="8449" width="14.81640625" customWidth="1"/>
+    <col min="8449" max="8449" width="14.85546875" customWidth="1"/>
     <col min="8450" max="8450" width="12" customWidth="1"/>
-    <col min="8451" max="8451" width="18.54296875" customWidth="1"/>
-    <col min="8452" max="8452" width="20.54296875" customWidth="1"/>
-    <col min="8453" max="8453" width="9.54296875" customWidth="1"/>
-    <col min="8454" max="8454" width="41.1796875" customWidth="1"/>
-    <col min="8455" max="8455" width="13.7265625" customWidth="1"/>
-    <col min="8456" max="8456" width="4.81640625" customWidth="1"/>
+    <col min="8451" max="8451" width="18.5703125" customWidth="1"/>
+    <col min="8452" max="8452" width="20.5703125" customWidth="1"/>
+    <col min="8453" max="8453" width="9.5703125" customWidth="1"/>
+    <col min="8454" max="8454" width="41.140625" customWidth="1"/>
+    <col min="8455" max="8455" width="13.7109375" customWidth="1"/>
+    <col min="8456" max="8456" width="4.85546875" customWidth="1"/>
     <col min="8457" max="8457" width="0" hidden="1" customWidth="1"/>
     <col min="8458" max="8458" width="29" customWidth="1"/>
-    <col min="8705" max="8705" width="14.81640625" customWidth="1"/>
+    <col min="8705" max="8705" width="14.85546875" customWidth="1"/>
     <col min="8706" max="8706" width="12" customWidth="1"/>
-    <col min="8707" max="8707" width="18.54296875" customWidth="1"/>
-    <col min="8708" max="8708" width="20.54296875" customWidth="1"/>
-    <col min="8709" max="8709" width="9.54296875" customWidth="1"/>
-    <col min="8710" max="8710" width="41.1796875" customWidth="1"/>
-    <col min="8711" max="8711" width="13.7265625" customWidth="1"/>
-    <col min="8712" max="8712" width="4.81640625" customWidth="1"/>
+    <col min="8707" max="8707" width="18.5703125" customWidth="1"/>
+    <col min="8708" max="8708" width="20.5703125" customWidth="1"/>
+    <col min="8709" max="8709" width="9.5703125" customWidth="1"/>
+    <col min="8710" max="8710" width="41.140625" customWidth="1"/>
+    <col min="8711" max="8711" width="13.7109375" customWidth="1"/>
+    <col min="8712" max="8712" width="4.85546875" customWidth="1"/>
     <col min="8713" max="8713" width="0" hidden="1" customWidth="1"/>
     <col min="8714" max="8714" width="29" customWidth="1"/>
-    <col min="8961" max="8961" width="14.81640625" customWidth="1"/>
+    <col min="8961" max="8961" width="14.85546875" customWidth="1"/>
     <col min="8962" max="8962" width="12" customWidth="1"/>
-    <col min="8963" max="8963" width="18.54296875" customWidth="1"/>
-    <col min="8964" max="8964" width="20.54296875" customWidth="1"/>
-    <col min="8965" max="8965" width="9.54296875" customWidth="1"/>
-    <col min="8966" max="8966" width="41.1796875" customWidth="1"/>
-    <col min="8967" max="8967" width="13.7265625" customWidth="1"/>
-    <col min="8968" max="8968" width="4.81640625" customWidth="1"/>
+    <col min="8963" max="8963" width="18.5703125" customWidth="1"/>
+    <col min="8964" max="8964" width="20.5703125" customWidth="1"/>
+    <col min="8965" max="8965" width="9.5703125" customWidth="1"/>
+    <col min="8966" max="8966" width="41.140625" customWidth="1"/>
+    <col min="8967" max="8967" width="13.7109375" customWidth="1"/>
+    <col min="8968" max="8968" width="4.85546875" customWidth="1"/>
     <col min="8969" max="8969" width="0" hidden="1" customWidth="1"/>
     <col min="8970" max="8970" width="29" customWidth="1"/>
-    <col min="9217" max="9217" width="14.81640625" customWidth="1"/>
+    <col min="9217" max="9217" width="14.85546875" customWidth="1"/>
     <col min="9218" max="9218" width="12" customWidth="1"/>
-    <col min="9219" max="9219" width="18.54296875" customWidth="1"/>
-    <col min="9220" max="9220" width="20.54296875" customWidth="1"/>
-    <col min="9221" max="9221" width="9.54296875" customWidth="1"/>
-    <col min="9222" max="9222" width="41.1796875" customWidth="1"/>
-    <col min="9223" max="9223" width="13.7265625" customWidth="1"/>
-    <col min="9224" max="9224" width="4.81640625" customWidth="1"/>
+    <col min="9219" max="9219" width="18.5703125" customWidth="1"/>
+    <col min="9220" max="9220" width="20.5703125" customWidth="1"/>
+    <col min="9221" max="9221" width="9.5703125" customWidth="1"/>
+    <col min="9222" max="9222" width="41.140625" customWidth="1"/>
+    <col min="9223" max="9223" width="13.7109375" customWidth="1"/>
+    <col min="9224" max="9224" width="4.85546875" customWidth="1"/>
     <col min="9225" max="9225" width="0" hidden="1" customWidth="1"/>
     <col min="9226" max="9226" width="29" customWidth="1"/>
-    <col min="9473" max="9473" width="14.81640625" customWidth="1"/>
+    <col min="9473" max="9473" width="14.85546875" customWidth="1"/>
     <col min="9474" max="9474" width="12" customWidth="1"/>
-    <col min="9475" max="9475" width="18.54296875" customWidth="1"/>
-    <col min="9476" max="9476" width="20.54296875" customWidth="1"/>
-    <col min="9477" max="9477" width="9.54296875" customWidth="1"/>
-    <col min="9478" max="9478" width="41.1796875" customWidth="1"/>
-    <col min="9479" max="9479" width="13.7265625" customWidth="1"/>
-    <col min="9480" max="9480" width="4.81640625" customWidth="1"/>
+    <col min="9475" max="9475" width="18.5703125" customWidth="1"/>
+    <col min="9476" max="9476" width="20.5703125" customWidth="1"/>
+    <col min="9477" max="9477" width="9.5703125" customWidth="1"/>
+    <col min="9478" max="9478" width="41.140625" customWidth="1"/>
+    <col min="9479" max="9479" width="13.7109375" customWidth="1"/>
+    <col min="9480" max="9480" width="4.85546875" customWidth="1"/>
     <col min="9481" max="9481" width="0" hidden="1" customWidth="1"/>
     <col min="9482" max="9482" width="29" customWidth="1"/>
-    <col min="9729" max="9729" width="14.81640625" customWidth="1"/>
+    <col min="9729" max="9729" width="14.85546875" customWidth="1"/>
     <col min="9730" max="9730" width="12" customWidth="1"/>
-    <col min="9731" max="9731" width="18.54296875" customWidth="1"/>
-    <col min="9732" max="9732" width="20.54296875" customWidth="1"/>
-    <col min="9733" max="9733" width="9.54296875" customWidth="1"/>
-    <col min="9734" max="9734" width="41.1796875" customWidth="1"/>
-    <col min="9735" max="9735" width="13.7265625" customWidth="1"/>
-    <col min="9736" max="9736" width="4.81640625" customWidth="1"/>
+    <col min="9731" max="9731" width="18.5703125" customWidth="1"/>
+    <col min="9732" max="9732" width="20.5703125" customWidth="1"/>
+    <col min="9733" max="9733" width="9.5703125" customWidth="1"/>
+    <col min="9734" max="9734" width="41.140625" customWidth="1"/>
+    <col min="9735" max="9735" width="13.7109375" customWidth="1"/>
+    <col min="9736" max="9736" width="4.85546875" customWidth="1"/>
     <col min="9737" max="9737" width="0" hidden="1" customWidth="1"/>
     <col min="9738" max="9738" width="29" customWidth="1"/>
-    <col min="9985" max="9985" width="14.81640625" customWidth="1"/>
+    <col min="9985" max="9985" width="14.85546875" customWidth="1"/>
     <col min="9986" max="9986" width="12" customWidth="1"/>
-    <col min="9987" max="9987" width="18.54296875" customWidth="1"/>
-    <col min="9988" max="9988" width="20.54296875" customWidth="1"/>
-    <col min="9989" max="9989" width="9.54296875" customWidth="1"/>
-    <col min="9990" max="9990" width="41.1796875" customWidth="1"/>
-    <col min="9991" max="9991" width="13.7265625" customWidth="1"/>
-    <col min="9992" max="9992" width="4.81640625" customWidth="1"/>
+    <col min="9987" max="9987" width="18.5703125" customWidth="1"/>
+    <col min="9988" max="9988" width="20.5703125" customWidth="1"/>
+    <col min="9989" max="9989" width="9.5703125" customWidth="1"/>
+    <col min="9990" max="9990" width="41.140625" customWidth="1"/>
+    <col min="9991" max="9991" width="13.7109375" customWidth="1"/>
+    <col min="9992" max="9992" width="4.85546875" customWidth="1"/>
     <col min="9993" max="9993" width="0" hidden="1" customWidth="1"/>
     <col min="9994" max="9994" width="29" customWidth="1"/>
-    <col min="10241" max="10241" width="14.81640625" customWidth="1"/>
+    <col min="10241" max="10241" width="14.85546875" customWidth="1"/>
     <col min="10242" max="10242" width="12" customWidth="1"/>
-    <col min="10243" max="10243" width="18.54296875" customWidth="1"/>
-    <col min="10244" max="10244" width="20.54296875" customWidth="1"/>
-    <col min="10245" max="10245" width="9.54296875" customWidth="1"/>
-    <col min="10246" max="10246" width="41.1796875" customWidth="1"/>
-    <col min="10247" max="10247" width="13.7265625" customWidth="1"/>
-    <col min="10248" max="10248" width="4.81640625" customWidth="1"/>
+    <col min="10243" max="10243" width="18.5703125" customWidth="1"/>
+    <col min="10244" max="10244" width="20.5703125" customWidth="1"/>
+    <col min="10245" max="10245" width="9.5703125" customWidth="1"/>
+    <col min="10246" max="10246" width="41.140625" customWidth="1"/>
+    <col min="10247" max="10247" width="13.7109375" customWidth="1"/>
+    <col min="10248" max="10248" width="4.85546875" customWidth="1"/>
     <col min="10249" max="10249" width="0" hidden="1" customWidth="1"/>
     <col min="10250" max="10250" width="29" customWidth="1"/>
-    <col min="10497" max="10497" width="14.81640625" customWidth="1"/>
+    <col min="10497" max="10497" width="14.85546875" customWidth="1"/>
     <col min="10498" max="10498" width="12" customWidth="1"/>
-    <col min="10499" max="10499" width="18.54296875" customWidth="1"/>
-    <col min="10500" max="10500" width="20.54296875" customWidth="1"/>
-    <col min="10501" max="10501" width="9.54296875" customWidth="1"/>
-    <col min="10502" max="10502" width="41.1796875" customWidth="1"/>
-    <col min="10503" max="10503" width="13.7265625" customWidth="1"/>
-    <col min="10504" max="10504" width="4.81640625" customWidth="1"/>
+    <col min="10499" max="10499" width="18.5703125" customWidth="1"/>
+    <col min="10500" max="10500" width="20.5703125" customWidth="1"/>
+    <col min="10501" max="10501" width="9.5703125" customWidth="1"/>
+    <col min="10502" max="10502" width="41.140625" customWidth="1"/>
+    <col min="10503" max="10503" width="13.7109375" customWidth="1"/>
+    <col min="10504" max="10504" width="4.85546875" customWidth="1"/>
     <col min="10505" max="10505" width="0" hidden="1" customWidth="1"/>
     <col min="10506" max="10506" width="29" customWidth="1"/>
-    <col min="10753" max="10753" width="14.81640625" customWidth="1"/>
+    <col min="10753" max="10753" width="14.85546875" customWidth="1"/>
     <col min="10754" max="10754" width="12" customWidth="1"/>
-    <col min="10755" max="10755" width="18.54296875" customWidth="1"/>
-    <col min="10756" max="10756" width="20.54296875" customWidth="1"/>
-    <col min="10757" max="10757" width="9.54296875" customWidth="1"/>
-    <col min="10758" max="10758" width="41.1796875" customWidth="1"/>
-    <col min="10759" max="10759" width="13.7265625" customWidth="1"/>
-    <col min="10760" max="10760" width="4.81640625" customWidth="1"/>
+    <col min="10755" max="10755" width="18.5703125" customWidth="1"/>
+    <col min="10756" max="10756" width="20.5703125" customWidth="1"/>
+    <col min="10757" max="10757" width="9.5703125" customWidth="1"/>
+    <col min="10758" max="10758" width="41.140625" customWidth="1"/>
+    <col min="10759" max="10759" width="13.7109375" customWidth="1"/>
+    <col min="10760" max="10760" width="4.85546875" customWidth="1"/>
     <col min="10761" max="10761" width="0" hidden="1" customWidth="1"/>
     <col min="10762" max="10762" width="29" customWidth="1"/>
-    <col min="11009" max="11009" width="14.81640625" customWidth="1"/>
+    <col min="11009" max="11009" width="14.85546875" customWidth="1"/>
     <col min="11010" max="11010" width="12" customWidth="1"/>
-    <col min="11011" max="11011" width="18.54296875" customWidth="1"/>
-    <col min="11012" max="11012" width="20.54296875" customWidth="1"/>
-    <col min="11013" max="11013" width="9.54296875" customWidth="1"/>
-    <col min="11014" max="11014" width="41.1796875" customWidth="1"/>
-    <col min="11015" max="11015" width="13.7265625" customWidth="1"/>
-    <col min="11016" max="11016" width="4.81640625" customWidth="1"/>
+    <col min="11011" max="11011" width="18.5703125" customWidth="1"/>
+    <col min="11012" max="11012" width="20.5703125" customWidth="1"/>
+    <col min="11013" max="11013" width="9.5703125" customWidth="1"/>
+    <col min="11014" max="11014" width="41.140625" customWidth="1"/>
+    <col min="11015" max="11015" width="13.7109375" customWidth="1"/>
+    <col min="11016" max="11016" width="4.85546875" customWidth="1"/>
     <col min="11017" max="11017" width="0" hidden="1" customWidth="1"/>
     <col min="11018" max="11018" width="29" customWidth="1"/>
-    <col min="11265" max="11265" width="14.81640625" customWidth="1"/>
+    <col min="11265" max="11265" width="14.85546875" customWidth="1"/>
     <col min="11266" max="11266" width="12" customWidth="1"/>
-    <col min="11267" max="11267" width="18.54296875" customWidth="1"/>
-    <col min="11268" max="11268" width="20.54296875" customWidth="1"/>
-    <col min="11269" max="11269" width="9.54296875" customWidth="1"/>
-    <col min="11270" max="11270" width="41.1796875" customWidth="1"/>
-    <col min="11271" max="11271" width="13.7265625" customWidth="1"/>
-    <col min="11272" max="11272" width="4.81640625" customWidth="1"/>
+    <col min="11267" max="11267" width="18.5703125" customWidth="1"/>
+    <col min="11268" max="11268" width="20.5703125" customWidth="1"/>
+    <col min="11269" max="11269" width="9.5703125" customWidth="1"/>
+    <col min="11270" max="11270" width="41.140625" customWidth="1"/>
+    <col min="11271" max="11271" width="13.7109375" customWidth="1"/>
+    <col min="11272" max="11272" width="4.85546875" customWidth="1"/>
     <col min="11273" max="11273" width="0" hidden="1" customWidth="1"/>
     <col min="11274" max="11274" width="29" customWidth="1"/>
-    <col min="11521" max="11521" width="14.81640625" customWidth="1"/>
+    <col min="11521" max="11521" width="14.85546875" customWidth="1"/>
     <col min="11522" max="11522" width="12" customWidth="1"/>
-    <col min="11523" max="11523" width="18.54296875" customWidth="1"/>
-    <col min="11524" max="11524" width="20.54296875" customWidth="1"/>
-    <col min="11525" max="11525" width="9.54296875" customWidth="1"/>
-    <col min="11526" max="11526" width="41.1796875" customWidth="1"/>
-    <col min="11527" max="11527" width="13.7265625" customWidth="1"/>
-    <col min="11528" max="11528" width="4.81640625" customWidth="1"/>
+    <col min="11523" max="11523" width="18.5703125" customWidth="1"/>
+    <col min="11524" max="11524" width="20.5703125" customWidth="1"/>
+    <col min="11525" max="11525" width="9.5703125" customWidth="1"/>
+    <col min="11526" max="11526" width="41.140625" customWidth="1"/>
+    <col min="11527" max="11527" width="13.7109375" customWidth="1"/>
+    <col min="11528" max="11528" width="4.85546875" customWidth="1"/>
     <col min="11529" max="11529" width="0" hidden="1" customWidth="1"/>
     <col min="11530" max="11530" width="29" customWidth="1"/>
-    <col min="11777" max="11777" width="14.81640625" customWidth="1"/>
+    <col min="11777" max="11777" width="14.85546875" customWidth="1"/>
     <col min="11778" max="11778" width="12" customWidth="1"/>
-    <col min="11779" max="11779" width="18.54296875" customWidth="1"/>
-    <col min="11780" max="11780" width="20.54296875" customWidth="1"/>
-    <col min="11781" max="11781" width="9.54296875" customWidth="1"/>
-    <col min="11782" max="11782" width="41.1796875" customWidth="1"/>
-    <col min="11783" max="11783" width="13.7265625" customWidth="1"/>
-    <col min="11784" max="11784" width="4.81640625" customWidth="1"/>
+    <col min="11779" max="11779" width="18.5703125" customWidth="1"/>
+    <col min="11780" max="11780" width="20.5703125" customWidth="1"/>
+    <col min="11781" max="11781" width="9.5703125" customWidth="1"/>
+    <col min="11782" max="11782" width="41.140625" customWidth="1"/>
+    <col min="11783" max="11783" width="13.7109375" customWidth="1"/>
+    <col min="11784" max="11784" width="4.85546875" customWidth="1"/>
     <col min="11785" max="11785" width="0" hidden="1" customWidth="1"/>
     <col min="11786" max="11786" width="29" customWidth="1"/>
-    <col min="12033" max="12033" width="14.81640625" customWidth="1"/>
+    <col min="12033" max="12033" width="14.85546875" customWidth="1"/>
     <col min="12034" max="12034" width="12" customWidth="1"/>
-    <col min="12035" max="12035" width="18.54296875" customWidth="1"/>
-    <col min="12036" max="12036" width="20.54296875" customWidth="1"/>
-    <col min="12037" max="12037" width="9.54296875" customWidth="1"/>
-    <col min="12038" max="12038" width="41.1796875" customWidth="1"/>
-    <col min="12039" max="12039" width="13.7265625" customWidth="1"/>
-    <col min="12040" max="12040" width="4.81640625" customWidth="1"/>
+    <col min="12035" max="12035" width="18.5703125" customWidth="1"/>
+    <col min="12036" max="12036" width="20.5703125" customWidth="1"/>
+    <col min="12037" max="12037" width="9.5703125" customWidth="1"/>
+    <col min="12038" max="12038" width="41.140625" customWidth="1"/>
+    <col min="12039" max="12039" width="13.7109375" customWidth="1"/>
+    <col min="12040" max="12040" width="4.85546875" customWidth="1"/>
     <col min="12041" max="12041" width="0" hidden="1" customWidth="1"/>
     <col min="12042" max="12042" width="29" customWidth="1"/>
-    <col min="12289" max="12289" width="14.81640625" customWidth="1"/>
+    <col min="12289" max="12289" width="14.85546875" customWidth="1"/>
     <col min="12290" max="12290" width="12" customWidth="1"/>
-    <col min="12291" max="12291" width="18.54296875" customWidth="1"/>
-    <col min="12292" max="12292" width="20.54296875" customWidth="1"/>
-    <col min="12293" max="12293" width="9.54296875" customWidth="1"/>
-    <col min="12294" max="12294" width="41.1796875" customWidth="1"/>
-    <col min="12295" max="12295" width="13.7265625" customWidth="1"/>
-    <col min="12296" max="12296" width="4.81640625" customWidth="1"/>
+    <col min="12291" max="12291" width="18.5703125" customWidth="1"/>
+    <col min="12292" max="12292" width="20.5703125" customWidth="1"/>
+    <col min="12293" max="12293" width="9.5703125" customWidth="1"/>
+    <col min="12294" max="12294" width="41.140625" customWidth="1"/>
+    <col min="12295" max="12295" width="13.7109375" customWidth="1"/>
+    <col min="12296" max="12296" width="4.85546875" customWidth="1"/>
     <col min="12297" max="12297" width="0" hidden="1" customWidth="1"/>
     <col min="12298" max="12298" width="29" customWidth="1"/>
-    <col min="12545" max="12545" width="14.81640625" customWidth="1"/>
+    <col min="12545" max="12545" width="14.85546875" customWidth="1"/>
     <col min="12546" max="12546" width="12" customWidth="1"/>
-    <col min="12547" max="12547" width="18.54296875" customWidth="1"/>
-    <col min="12548" max="12548" width="20.54296875" customWidth="1"/>
-    <col min="12549" max="12549" width="9.54296875" customWidth="1"/>
-    <col min="12550" max="12550" width="41.1796875" customWidth="1"/>
-    <col min="12551" max="12551" width="13.7265625" customWidth="1"/>
-    <col min="12552" max="12552" width="4.81640625" customWidth="1"/>
+    <col min="12547" max="12547" width="18.5703125" customWidth="1"/>
+    <col min="12548" max="12548" width="20.5703125" customWidth="1"/>
+    <col min="12549" max="12549" width="9.5703125" customWidth="1"/>
+    <col min="12550" max="12550" width="41.140625" customWidth="1"/>
+    <col min="12551" max="12551" width="13.7109375" customWidth="1"/>
+    <col min="12552" max="12552" width="4.85546875" customWidth="1"/>
     <col min="12553" max="12553" width="0" hidden="1" customWidth="1"/>
     <col min="12554" max="12554" width="29" customWidth="1"/>
-    <col min="12801" max="12801" width="14.81640625" customWidth="1"/>
+    <col min="12801" max="12801" width="14.85546875" customWidth="1"/>
     <col min="12802" max="12802" width="12" customWidth="1"/>
-    <col min="12803" max="12803" width="18.54296875" customWidth="1"/>
-    <col min="12804" max="12804" width="20.54296875" customWidth="1"/>
-    <col min="12805" max="12805" width="9.54296875" customWidth="1"/>
-    <col min="12806" max="12806" width="41.1796875" customWidth="1"/>
-    <col min="12807" max="12807" width="13.7265625" customWidth="1"/>
-    <col min="12808" max="12808" width="4.81640625" customWidth="1"/>
+    <col min="12803" max="12803" width="18.5703125" customWidth="1"/>
+    <col min="12804" max="12804" width="20.5703125" customWidth="1"/>
+    <col min="12805" max="12805" width="9.5703125" customWidth="1"/>
+    <col min="12806" max="12806" width="41.140625" customWidth="1"/>
+    <col min="12807" max="12807" width="13.7109375" customWidth="1"/>
+    <col min="12808" max="12808" width="4.85546875" customWidth="1"/>
     <col min="12809" max="12809" width="0" hidden="1" customWidth="1"/>
     <col min="12810" max="12810" width="29" customWidth="1"/>
-    <col min="13057" max="13057" width="14.81640625" customWidth="1"/>
+    <col min="13057" max="13057" width="14.85546875" customWidth="1"/>
     <col min="13058" max="13058" width="12" customWidth="1"/>
-    <col min="13059" max="13059" width="18.54296875" customWidth="1"/>
-    <col min="13060" max="13060" width="20.54296875" customWidth="1"/>
-    <col min="13061" max="13061" width="9.54296875" customWidth="1"/>
-    <col min="13062" max="13062" width="41.1796875" customWidth="1"/>
-    <col min="13063" max="13063" width="13.7265625" customWidth="1"/>
-    <col min="13064" max="13064" width="4.81640625" customWidth="1"/>
+    <col min="13059" max="13059" width="18.5703125" customWidth="1"/>
+    <col min="13060" max="13060" width="20.5703125" customWidth="1"/>
+    <col min="13061" max="13061" width="9.5703125" customWidth="1"/>
+    <col min="13062" max="13062" width="41.140625" customWidth="1"/>
+    <col min="13063" max="13063" width="13.7109375" customWidth="1"/>
+    <col min="13064" max="13064" width="4.85546875" customWidth="1"/>
     <col min="13065" max="13065" width="0" hidden="1" customWidth="1"/>
     <col min="13066" max="13066" width="29" customWidth="1"/>
-    <col min="13313" max="13313" width="14.81640625" customWidth="1"/>
+    <col min="13313" max="13313" width="14.85546875" customWidth="1"/>
     <col min="13314" max="13314" width="12" customWidth="1"/>
-    <col min="13315" max="13315" width="18.54296875" customWidth="1"/>
-    <col min="13316" max="13316" width="20.54296875" customWidth="1"/>
-    <col min="13317" max="13317" width="9.54296875" customWidth="1"/>
-    <col min="13318" max="13318" width="41.1796875" customWidth="1"/>
-    <col min="13319" max="13319" width="13.7265625" customWidth="1"/>
-    <col min="13320" max="13320" width="4.81640625" customWidth="1"/>
+    <col min="13315" max="13315" width="18.5703125" customWidth="1"/>
+    <col min="13316" max="13316" width="20.5703125" customWidth="1"/>
+    <col min="13317" max="13317" width="9.5703125" customWidth="1"/>
+    <col min="13318" max="13318" width="41.140625" customWidth="1"/>
+    <col min="13319" max="13319" width="13.7109375" customWidth="1"/>
+    <col min="13320" max="13320" width="4.85546875" customWidth="1"/>
     <col min="13321" max="13321" width="0" hidden="1" customWidth="1"/>
     <col min="13322" max="13322" width="29" customWidth="1"/>
-    <col min="13569" max="13569" width="14.81640625" customWidth="1"/>
+    <col min="13569" max="13569" width="14.85546875" customWidth="1"/>
     <col min="13570" max="13570" width="12" customWidth="1"/>
-    <col min="13571" max="13571" width="18.54296875" customWidth="1"/>
-    <col min="13572" max="13572" width="20.54296875" customWidth="1"/>
-    <col min="13573" max="13573" width="9.54296875" customWidth="1"/>
-    <col min="13574" max="13574" width="41.1796875" customWidth="1"/>
-    <col min="13575" max="13575" width="13.7265625" customWidth="1"/>
-    <col min="13576" max="13576" width="4.81640625" customWidth="1"/>
+    <col min="13571" max="13571" width="18.5703125" customWidth="1"/>
+    <col min="13572" max="13572" width="20.5703125" customWidth="1"/>
+    <col min="13573" max="13573" width="9.5703125" customWidth="1"/>
+    <col min="13574" max="13574" width="41.140625" customWidth="1"/>
+    <col min="13575" max="13575" width="13.7109375" customWidth="1"/>
+    <col min="13576" max="13576" width="4.85546875" customWidth="1"/>
     <col min="13577" max="13577" width="0" hidden="1" customWidth="1"/>
     <col min="13578" max="13578" width="29" customWidth="1"/>
-    <col min="13825" max="13825" width="14.81640625" customWidth="1"/>
+    <col min="13825" max="13825" width="14.85546875" customWidth="1"/>
     <col min="13826" max="13826" width="12" customWidth="1"/>
-    <col min="13827" max="13827" width="18.54296875" customWidth="1"/>
-    <col min="13828" max="13828" width="20.54296875" customWidth="1"/>
-    <col min="13829" max="13829" width="9.54296875" customWidth="1"/>
-    <col min="13830" max="13830" width="41.1796875" customWidth="1"/>
-    <col min="13831" max="13831" width="13.7265625" customWidth="1"/>
-    <col min="13832" max="13832" width="4.81640625" customWidth="1"/>
+    <col min="13827" max="13827" width="18.5703125" customWidth="1"/>
+    <col min="13828" max="13828" width="20.5703125" customWidth="1"/>
+    <col min="13829" max="13829" width="9.5703125" customWidth="1"/>
+    <col min="13830" max="13830" width="41.140625" customWidth="1"/>
+    <col min="13831" max="13831" width="13.7109375" customWidth="1"/>
+    <col min="13832" max="13832" width="4.85546875" customWidth="1"/>
     <col min="13833" max="13833" width="0" hidden="1" customWidth="1"/>
     <col min="13834" max="13834" width="29" customWidth="1"/>
-    <col min="14081" max="14081" width="14.81640625" customWidth="1"/>
+    <col min="14081" max="14081" width="14.85546875" customWidth="1"/>
     <col min="14082" max="14082" width="12" customWidth="1"/>
-    <col min="14083" max="14083" width="18.54296875" customWidth="1"/>
-    <col min="14084" max="14084" width="20.54296875" customWidth="1"/>
-    <col min="14085" max="14085" width="9.54296875" customWidth="1"/>
-    <col min="14086" max="14086" width="41.1796875" customWidth="1"/>
-    <col min="14087" max="14087" width="13.7265625" customWidth="1"/>
-    <col min="14088" max="14088" width="4.81640625" customWidth="1"/>
+    <col min="14083" max="14083" width="18.5703125" customWidth="1"/>
+    <col min="14084" max="14084" width="20.5703125" customWidth="1"/>
+    <col min="14085" max="14085" width="9.5703125" customWidth="1"/>
+    <col min="14086" max="14086" width="41.140625" customWidth="1"/>
+    <col min="14087" max="14087" width="13.7109375" customWidth="1"/>
+    <col min="14088" max="14088" width="4.85546875" customWidth="1"/>
     <col min="14089" max="14089" width="0" hidden="1" customWidth="1"/>
     <col min="14090" max="14090" width="29" customWidth="1"/>
-    <col min="14337" max="14337" width="14.81640625" customWidth="1"/>
+    <col min="14337" max="14337" width="14.85546875" customWidth="1"/>
     <col min="14338" max="14338" width="12" customWidth="1"/>
-    <col min="14339" max="14339" width="18.54296875" customWidth="1"/>
-    <col min="14340" max="14340" width="20.54296875" customWidth="1"/>
-    <col min="14341" max="14341" width="9.54296875" customWidth="1"/>
-    <col min="14342" max="14342" width="41.1796875" customWidth="1"/>
-    <col min="14343" max="14343" width="13.7265625" customWidth="1"/>
-    <col min="14344" max="14344" width="4.81640625" customWidth="1"/>
+    <col min="14339" max="14339" width="18.5703125" customWidth="1"/>
+    <col min="14340" max="14340" width="20.5703125" customWidth="1"/>
+    <col min="14341" max="14341" width="9.5703125" customWidth="1"/>
+    <col min="14342" max="14342" width="41.140625" customWidth="1"/>
+    <col min="14343" max="14343" width="13.7109375" customWidth="1"/>
+    <col min="14344" max="14344" width="4.85546875" customWidth="1"/>
     <col min="14345" max="14345" width="0" hidden="1" customWidth="1"/>
     <col min="14346" max="14346" width="29" customWidth="1"/>
-    <col min="14593" max="14593" width="14.81640625" customWidth="1"/>
+    <col min="14593" max="14593" width="14.85546875" customWidth="1"/>
     <col min="14594" max="14594" width="12" customWidth="1"/>
-    <col min="14595" max="14595" width="18.54296875" customWidth="1"/>
-    <col min="14596" max="14596" width="20.54296875" customWidth="1"/>
-    <col min="14597" max="14597" width="9.54296875" customWidth="1"/>
-    <col min="14598" max="14598" width="41.1796875" customWidth="1"/>
-    <col min="14599" max="14599" width="13.7265625" customWidth="1"/>
-    <col min="14600" max="14600" width="4.81640625" customWidth="1"/>
+    <col min="14595" max="14595" width="18.5703125" customWidth="1"/>
+    <col min="14596" max="14596" width="20.5703125" customWidth="1"/>
+    <col min="14597" max="14597" width="9.5703125" customWidth="1"/>
+    <col min="14598" max="14598" width="41.140625" customWidth="1"/>
+    <col min="14599" max="14599" width="13.7109375" customWidth="1"/>
+    <col min="14600" max="14600" width="4.85546875" customWidth="1"/>
     <col min="14601" max="14601" width="0" hidden="1" customWidth="1"/>
     <col min="14602" max="14602" width="29" customWidth="1"/>
-    <col min="14849" max="14849" width="14.81640625" customWidth="1"/>
+    <col min="14849" max="14849" width="14.85546875" customWidth="1"/>
     <col min="14850" max="14850" width="12" customWidth="1"/>
-    <col min="14851" max="14851" width="18.54296875" customWidth="1"/>
-    <col min="14852" max="14852" width="20.54296875" customWidth="1"/>
-    <col min="14853" max="14853" width="9.54296875" customWidth="1"/>
-    <col min="14854" max="14854" width="41.1796875" customWidth="1"/>
-    <col min="14855" max="14855" width="13.7265625" customWidth="1"/>
-    <col min="14856" max="14856" width="4.81640625" customWidth="1"/>
+    <col min="14851" max="14851" width="18.5703125" customWidth="1"/>
+    <col min="14852" max="14852" width="20.5703125" customWidth="1"/>
+    <col min="14853" max="14853" width="9.5703125" customWidth="1"/>
+    <col min="14854" max="14854" width="41.140625" customWidth="1"/>
+    <col min="14855" max="14855" width="13.7109375" customWidth="1"/>
+    <col min="14856" max="14856" width="4.85546875" customWidth="1"/>
     <col min="14857" max="14857" width="0" hidden="1" customWidth="1"/>
     <col min="14858" max="14858" width="29" customWidth="1"/>
-    <col min="15105" max="15105" width="14.81640625" customWidth="1"/>
+    <col min="15105" max="15105" width="14.85546875" customWidth="1"/>
     <col min="15106" max="15106" width="12" customWidth="1"/>
-    <col min="15107" max="15107" width="18.54296875" customWidth="1"/>
-    <col min="15108" max="15108" width="20.54296875" customWidth="1"/>
-    <col min="15109" max="15109" width="9.54296875" customWidth="1"/>
-    <col min="15110" max="15110" width="41.1796875" customWidth="1"/>
-    <col min="15111" max="15111" width="13.7265625" customWidth="1"/>
-    <col min="15112" max="15112" width="4.81640625" customWidth="1"/>
+    <col min="15107" max="15107" width="18.5703125" customWidth="1"/>
+    <col min="15108" max="15108" width="20.5703125" customWidth="1"/>
+    <col min="15109" max="15109" width="9.5703125" customWidth="1"/>
+    <col min="15110" max="15110" width="41.140625" customWidth="1"/>
+    <col min="15111" max="15111" width="13.7109375" customWidth="1"/>
+    <col min="15112" max="15112" width="4.85546875" customWidth="1"/>
     <col min="15113" max="15113" width="0" hidden="1" customWidth="1"/>
     <col min="15114" max="15114" width="29" customWidth="1"/>
-    <col min="15361" max="15361" width="14.81640625" customWidth="1"/>
+    <col min="15361" max="15361" width="14.85546875" customWidth="1"/>
     <col min="15362" max="15362" width="12" customWidth="1"/>
-    <col min="15363" max="15363" width="18.54296875" customWidth="1"/>
-    <col min="15364" max="15364" width="20.54296875" customWidth="1"/>
-    <col min="15365" max="15365" width="9.54296875" customWidth="1"/>
-    <col min="15366" max="15366" width="41.1796875" customWidth="1"/>
-    <col min="15367" max="15367" width="13.7265625" customWidth="1"/>
-    <col min="15368" max="15368" width="4.81640625" customWidth="1"/>
+    <col min="15363" max="15363" width="18.5703125" customWidth="1"/>
+    <col min="15364" max="15364" width="20.5703125" customWidth="1"/>
+    <col min="15365" max="15365" width="9.5703125" customWidth="1"/>
+    <col min="15366" max="15366" width="41.140625" customWidth="1"/>
+    <col min="15367" max="15367" width="13.7109375" customWidth="1"/>
+    <col min="15368" max="15368" width="4.85546875" customWidth="1"/>
     <col min="15369" max="15369" width="0" hidden="1" customWidth="1"/>
     <col min="15370" max="15370" width="29" customWidth="1"/>
-    <col min="15617" max="15617" width="14.81640625" customWidth="1"/>
+    <col min="15617" max="15617" width="14.85546875" customWidth="1"/>
     <col min="15618" max="15618" width="12" customWidth="1"/>
-    <col min="15619" max="15619" width="18.54296875" customWidth="1"/>
-    <col min="15620" max="15620" width="20.54296875" customWidth="1"/>
-    <col min="15621" max="15621" width="9.54296875" customWidth="1"/>
-    <col min="15622" max="15622" width="41.1796875" customWidth="1"/>
-    <col min="15623" max="15623" width="13.7265625" customWidth="1"/>
-    <col min="15624" max="15624" width="4.81640625" customWidth="1"/>
+    <col min="15619" max="15619" width="18.5703125" customWidth="1"/>
+    <col min="15620" max="15620" width="20.5703125" customWidth="1"/>
+    <col min="15621" max="15621" width="9.5703125" customWidth="1"/>
+    <col min="15622" max="15622" width="41.140625" customWidth="1"/>
+    <col min="15623" max="15623" width="13.7109375" customWidth="1"/>
+    <col min="15624" max="15624" width="4.85546875" customWidth="1"/>
     <col min="15625" max="15625" width="0" hidden="1" customWidth="1"/>
     <col min="15626" max="15626" width="29" customWidth="1"/>
-    <col min="15873" max="15873" width="14.81640625" customWidth="1"/>
+    <col min="15873" max="15873" width="14.85546875" customWidth="1"/>
     <col min="15874" max="15874" width="12" customWidth="1"/>
-    <col min="15875" max="15875" width="18.54296875" customWidth="1"/>
-    <col min="15876" max="15876" width="20.54296875" customWidth="1"/>
-    <col min="15877" max="15877" width="9.54296875" customWidth="1"/>
-    <col min="15878" max="15878" width="41.1796875" customWidth="1"/>
-    <col min="15879" max="15879" width="13.7265625" customWidth="1"/>
-    <col min="15880" max="15880" width="4.81640625" customWidth="1"/>
+    <col min="15875" max="15875" width="18.5703125" customWidth="1"/>
+    <col min="15876" max="15876" width="20.5703125" customWidth="1"/>
+    <col min="15877" max="15877" width="9.5703125" customWidth="1"/>
+    <col min="15878" max="15878" width="41.140625" customWidth="1"/>
+    <col min="15879" max="15879" width="13.7109375" customWidth="1"/>
+    <col min="15880" max="15880" width="4.85546875" customWidth="1"/>
     <col min="15881" max="15881" width="0" hidden="1" customWidth="1"/>
     <col min="15882" max="15882" width="29" customWidth="1"/>
-    <col min="16129" max="16129" width="14.81640625" customWidth="1"/>
+    <col min="16129" max="16129" width="14.85546875" customWidth="1"/>
     <col min="16130" max="16130" width="12" customWidth="1"/>
-    <col min="16131" max="16131" width="18.54296875" customWidth="1"/>
-    <col min="16132" max="16132" width="20.54296875" customWidth="1"/>
-    <col min="16133" max="16133" width="9.54296875" customWidth="1"/>
-    <col min="16134" max="16134" width="41.1796875" customWidth="1"/>
-    <col min="16135" max="16135" width="13.7265625" customWidth="1"/>
-    <col min="16136" max="16136" width="4.81640625" customWidth="1"/>
+    <col min="16131" max="16131" width="18.5703125" customWidth="1"/>
+    <col min="16132" max="16132" width="20.5703125" customWidth="1"/>
+    <col min="16133" max="16133" width="9.5703125" customWidth="1"/>
+    <col min="16134" max="16134" width="41.140625" customWidth="1"/>
+    <col min="16135" max="16135" width="13.7109375" customWidth="1"/>
+    <col min="16136" max="16136" width="4.85546875" customWidth="1"/>
     <col min="16137" max="16137" width="0" hidden="1" customWidth="1"/>
     <col min="16138" max="16138" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2732,7 +2735,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2754,7 +2757,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2820,7 +2823,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -2886,7 +2889,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2908,7 +2911,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -2930,7 +2933,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -2952,7 +2955,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -3040,7 +3043,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>75</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
@@ -3080,7 +3083,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>79</v>
       </c>
@@ -3100,7 +3103,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
@@ -3120,7 +3123,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>79</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>79</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>79</v>
       </c>
@@ -3178,7 +3181,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>79</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>100</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>100</v>
       </c>
@@ -3236,7 +3239,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>100</v>
       </c>
@@ -3256,7 +3259,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>100</v>
       </c>
@@ -3276,7 +3279,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>111</v>
       </c>
@@ -3296,7 +3299,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>111</v>
       </c>
@@ -3316,7 +3319,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>111</v>
       </c>
@@ -3334,7 +3337,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>111</v>
       </c>
@@ -3354,7 +3357,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>111</v>
       </c>
@@ -3374,7 +3377,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>111</v>
       </c>
@@ -3394,7 +3397,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>128</v>
       </c>
@@ -3414,7 +3417,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>132</v>
       </c>
@@ -3434,7 +3437,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>132</v>
       </c>
@@ -3454,7 +3457,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>138</v>
       </c>
@@ -3474,7 +3477,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>142</v>
       </c>
@@ -3494,7 +3497,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>142</v>
       </c>
@@ -3512,7 +3515,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>142</v>
       </c>
@@ -3530,7 +3533,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>150</v>
       </c>
@@ -3550,7 +3553,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>154</v>
       </c>
@@ -3570,7 +3573,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>157</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>157</v>
       </c>
@@ -3614,7 +3617,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>157</v>
       </c>
@@ -3634,7 +3637,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>157</v>
       </c>
@@ -3656,7 +3659,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>157</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>157</v>
       </c>
@@ -3700,7 +3703,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>157</v>
       </c>
@@ -3722,7 +3725,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>185</v>
       </c>
@@ -3744,7 +3747,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>185</v>
       </c>
@@ -3766,7 +3769,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>194</v>
       </c>
@@ -3788,7 +3791,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>194</v>
       </c>
@@ -3810,7 +3813,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>194</v>
       </c>
@@ -3832,7 +3835,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>207</v>
       </c>
@@ -3852,7 +3855,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>207</v>
       </c>
@@ -3874,7 +3877,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>207</v>
       </c>
@@ -3896,7 +3899,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>219</v>
       </c>
@@ -3920,7 +3923,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>219</v>
       </c>
@@ -3942,7 +3945,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>219</v>
       </c>
@@ -3964,7 +3967,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>219</v>
       </c>
@@ -3986,7 +3989,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>219</v>
       </c>
@@ -4006,7 +4009,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>219</v>
       </c>
@@ -4026,7 +4029,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>219</v>
       </c>
@@ -4046,7 +4049,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>219</v>
       </c>
@@ -4068,7 +4071,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>219</v>
       </c>
@@ -4090,7 +4093,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>251</v>
       </c>
@@ -4110,7 +4113,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>255</v>
       </c>
@@ -4130,7 +4133,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>259</v>
       </c>
@@ -4152,7 +4155,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>259</v>
       </c>
@@ -4174,7 +4177,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>259</v>
       </c>
@@ -4196,7 +4199,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>270</v>
       </c>
@@ -4218,7 +4221,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>270</v>
       </c>
@@ -4240,7 +4243,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>270</v>
       </c>
@@ -4262,7 +4265,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>270</v>
       </c>
@@ -4284,7 +4287,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>270</v>
       </c>
@@ -4304,7 +4307,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>270</v>
       </c>
@@ -4326,7 +4329,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>270</v>
       </c>
@@ -4348,7 +4351,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>270</v>
       </c>
@@ -4370,7 +4373,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>270</v>
       </c>
@@ -4392,7 +4395,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>270</v>
       </c>
@@ -4414,7 +4417,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>270</v>
       </c>
@@ -4436,7 +4439,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>270</v>
       </c>
@@ -4458,7 +4461,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>270</v>
       </c>
@@ -4480,7 +4483,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>270</v>
       </c>
@@ -4502,7 +4505,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>270</v>
       </c>
@@ -4524,7 +4527,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>270</v>
       </c>
@@ -4546,7 +4549,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>270</v>
       </c>
@@ -4566,7 +4569,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>270</v>
       </c>
@@ -4588,7 +4591,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>328</v>
       </c>
@@ -4608,7 +4611,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>328</v>
       </c>
@@ -4628,7 +4631,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>328</v>
       </c>
@@ -4648,7 +4651,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>338</v>
       </c>
@@ -4670,7 +4673,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>338</v>
       </c>
@@ -4692,7 +4695,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>338</v>
       </c>
@@ -4714,7 +4717,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>338</v>
       </c>
@@ -4732,7 +4735,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>338</v>
       </c>
@@ -4754,7 +4757,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>338</v>
       </c>
@@ -4772,7 +4775,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>338</v>
       </c>
@@ -4794,7 +4797,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>338</v>
       </c>
@@ -4814,7 +4817,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>366</v>
       </c>
@@ -4836,7 +4839,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>371</v>
       </c>
@@ -4852,7 +4855,7 @@
       </c>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>371</v>
       </c>
@@ -4868,7 +4871,7 @@
       </c>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>371</v>
       </c>
@@ -4886,7 +4889,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>371</v>
       </c>
@@ -4904,7 +4907,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>379</v>
       </c>
@@ -4924,7 +4927,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>379</v>
       </c>
@@ -4946,7 +4949,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>379</v>
       </c>
@@ -4968,7 +4971,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>379</v>
       </c>
@@ -4990,7 +4993,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>379</v>
       </c>
@@ -5012,7 +5015,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>379</v>
       </c>
@@ -5034,7 +5037,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>379</v>
       </c>
@@ -5056,7 +5059,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>379</v>
       </c>
@@ -5078,7 +5081,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>379</v>
       </c>
@@ -5100,7 +5103,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>379</v>
       </c>
@@ -5122,7 +5125,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>379</v>
       </c>
@@ -5142,7 +5145,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>379</v>
       </c>
@@ -5164,7 +5167,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>379</v>
       </c>
@@ -5186,7 +5189,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>379</v>
       </c>
@@ -5208,7 +5211,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>379</v>
       </c>
@@ -5230,7 +5233,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>379</v>
       </c>
@@ -5250,7 +5253,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>379</v>
       </c>
@@ -5272,7 +5275,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>379</v>
       </c>
@@ -5292,7 +5295,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>379</v>
       </c>
@@ -5314,7 +5317,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>379</v>
       </c>
@@ -5334,7 +5337,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>379</v>
       </c>
@@ -5354,7 +5357,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>379</v>
       </c>
@@ -5376,7 +5379,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>379</v>
       </c>
@@ -5398,7 +5401,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>379</v>
       </c>
@@ -5420,7 +5423,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>379</v>
       </c>
@@ -5442,7 +5445,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>379</v>
       </c>
@@ -5462,7 +5465,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>379</v>
       </c>
@@ -5482,7 +5485,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>379</v>
       </c>
@@ -5502,7 +5505,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>379</v>
       </c>
@@ -5524,7 +5527,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>379</v>
       </c>
@@ -5542,7 +5545,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>379</v>
       </c>
@@ -5564,7 +5567,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>379</v>
       </c>
@@ -5586,7 +5589,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>379</v>
       </c>
@@ -5608,7 +5611,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>379</v>
       </c>
@@ -5630,7 +5633,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>379</v>
       </c>
@@ -5652,7 +5655,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>379</v>
       </c>
@@ -5674,7 +5677,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>379</v>
       </c>
@@ -5696,7 +5699,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>510</v>
       </c>
@@ -5718,7 +5721,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>510</v>
       </c>
@@ -5740,7 +5743,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>517</v>
       </c>
@@ -5762,7 +5765,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>517</v>
       </c>
@@ -5782,7 +5785,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>517</v>
       </c>
@@ -5804,7 +5807,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>517</v>
       </c>
@@ -5824,7 +5827,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>517</v>
       </c>
@@ -5846,7 +5849,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>517</v>
       </c>
@@ -5868,7 +5871,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>538</v>
       </c>
@@ -5890,7 +5893,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>538</v>
       </c>
@@ -5912,7 +5915,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>546</v>
       </c>
@@ -5932,7 +5935,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="108" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:8" ht="108" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.25" footer="0.25"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -5940,4 +5943,19 @@
     <oddFooter>&amp;L&amp;C&amp;R</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:WVQ12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed issue with bad call numbers
fixed error handling for bad call numbers. Bad call numbers get sorted
to the bottom of the list now
</commit_message>
<xml_diff>
--- a/Macro File/daily rtf test.xlsx
+++ b/Macro File/daily rtf test.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Daily RTF report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -167,9 +167,6 @@
     <t>Epic,</t>
   </si>
   <si>
-    <t>CD MR BUCKCHE</t>
-  </si>
-  <si>
     <t>Buckcherry (Musical group)</t>
   </si>
   <si>
@@ -1674,6 +1671,9 @@
   </si>
   <si>
     <t>Debunk it! : how to stay sane in a world of misinformation</t>
+  </si>
+  <si>
+    <t>CD MRI BUCKCHE</t>
   </si>
 </sst>
 </file>
@@ -2016,8 +2016,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2894,17 +2894,17 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="H11" s="1">
         <v>2009</v>
@@ -2916,17 +2916,17 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="H12" s="1">
         <v>2011</v>
@@ -2938,17 +2938,17 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H13" s="1">
         <v>2011</v>
@@ -2960,17 +2960,17 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="H14" s="1">
         <v>2012</v>
@@ -2982,17 +2982,17 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H15" s="1">
         <v>2011</v>
@@ -3004,17 +3004,17 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="H16" s="1">
         <v>2009</v>
@@ -3026,17 +3026,17 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="H17" s="1">
         <v>1993</v>
@@ -3044,19 +3044,19 @@
     </row>
     <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="H18" s="1">
         <v>2010</v>
@@ -3064,19 +3064,19 @@
     </row>
     <row r="19" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="H19" s="1">
         <v>2000</v>
@@ -3084,19 +3084,19 @@
     </row>
     <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="H20" s="1">
         <v>2009</v>
@@ -3104,19 +3104,19 @@
     </row>
     <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="H21" s="1">
         <v>2011</v>
@@ -3124,19 +3124,19 @@
     </row>
     <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="H22" s="1">
         <v>2007</v>
@@ -3144,16 +3144,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1">
@@ -3162,19 +3162,19 @@
     </row>
     <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="H24" s="1">
         <v>1998</v>
@@ -3182,19 +3182,19 @@
     </row>
     <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="H25" s="1">
         <v>1995</v>
@@ -3202,19 +3202,19 @@
     </row>
     <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="H26" s="1">
         <v>2013</v>
@@ -3222,16 +3222,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1">
@@ -3240,19 +3240,19 @@
     </row>
     <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="H28" s="1">
         <v>2007</v>
@@ -3260,19 +3260,19 @@
     </row>
     <row r="29" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H29" s="1">
         <v>2012</v>
@@ -3280,19 +3280,19 @@
     </row>
     <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="H30" s="1">
         <v>2006</v>
@@ -3300,19 +3300,19 @@
     </row>
     <row r="31" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H31" s="1">
         <v>2008</v>
@@ -3320,16 +3320,16 @@
     </row>
     <row r="32" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1">
@@ -3338,19 +3338,19 @@
     </row>
     <row r="33" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="H33" s="1">
         <v>2009</v>
@@ -3358,19 +3358,19 @@
     </row>
     <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="H34" s="1">
         <v>2004</v>
@@ -3378,19 +3378,19 @@
     </row>
     <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="H35" s="1">
         <v>1999</v>
@@ -3398,19 +3398,19 @@
     </row>
     <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="H36" s="1">
         <v>2003</v>
@@ -3418,19 +3418,19 @@
     </row>
     <row r="37" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H37" s="1">
         <v>2010</v>
@@ -3438,19 +3438,19 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="H38" s="1">
         <v>2014</v>
@@ -3458,19 +3458,19 @@
     </row>
     <row r="39" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="H39" s="1">
         <v>2006</v>
@@ -3478,19 +3478,19 @@
     </row>
     <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="H40" s="1">
         <v>2011</v>
@@ -3498,16 +3498,16 @@
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1">
@@ -3516,16 +3516,16 @@
     </row>
     <row r="42" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1">
@@ -3534,19 +3534,19 @@
     </row>
     <row r="43" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="H43" s="1">
         <v>2006</v>
@@ -3554,19 +3554,19 @@
     </row>
     <row r="44" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H44" s="1">
         <v>2008</v>
@@ -3574,21 +3574,21 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="H45" s="1">
         <v>1978</v>
@@ -3596,21 +3596,21 @@
     </row>
     <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="H46" s="1">
         <v>2014</v>
@@ -3618,18 +3618,18 @@
     </row>
     <row r="47" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1">
@@ -3638,21 +3638,21 @@
     </row>
     <row r="48" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="H48" s="1">
         <v>2010</v>
@@ -3660,21 +3660,21 @@
     </row>
     <row r="49" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="H49" s="1">
         <v>2008</v>
@@ -3682,21 +3682,21 @@
     </row>
     <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="H50" s="1">
         <v>2012</v>
@@ -3704,21 +3704,21 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="H51" s="1">
         <v>2008</v>
@@ -3726,21 +3726,21 @@
     </row>
     <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="H52" s="1">
         <v>1991</v>
@@ -3748,21 +3748,21 @@
     </row>
     <row r="53" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="H53" s="1">
         <v>2003</v>
@@ -3770,21 +3770,21 @@
     </row>
     <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="H54" s="1">
         <v>1987</v>
@@ -3792,21 +3792,21 @@
     </row>
     <row r="55" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="H55" s="1">
         <v>2008</v>
@@ -3814,21 +3814,21 @@
     </row>
     <row r="56" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="H56" s="1">
         <v>2002</v>
@@ -3836,19 +3836,19 @@
     </row>
     <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="H57" s="1">
         <v>1973</v>
@@ -3856,21 +3856,21 @@
     </row>
     <row r="58" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="H58" s="1">
         <v>2011</v>
@@ -3878,21 +3878,21 @@
     </row>
     <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="H59" s="1">
         <v>2004</v>
@@ -3900,23 +3900,23 @@
     </row>
     <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="H60" s="1">
         <v>2003</v>
@@ -3924,21 +3924,21 @@
     </row>
     <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="H61" s="1">
         <v>2011</v>
@@ -3946,21 +3946,21 @@
     </row>
     <row r="62" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="H62" s="1">
         <v>2014</v>
@@ -3968,20 +3968,20 @@
     </row>
     <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1">
@@ -3990,18 +3990,18 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1">
@@ -4010,18 +4010,18 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1">
@@ -4030,18 +4030,18 @@
     </row>
     <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1">
@@ -4050,20 +4050,20 @@
     </row>
     <row r="67" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1">
@@ -4072,21 +4072,21 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="H68" s="1">
         <v>2012</v>
@@ -4094,18 +4094,18 @@
     </row>
     <row r="69" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1">
@@ -4114,18 +4114,18 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1">
@@ -4134,21 +4134,21 @@
     </row>
     <row r="71" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="H71" s="1">
         <v>2006</v>
@@ -4156,21 +4156,21 @@
     </row>
     <row r="72" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="H72" s="1">
         <v>2014</v>
@@ -4178,21 +4178,21 @@
     </row>
     <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H73" s="1">
         <v>1996</v>
@@ -4200,21 +4200,21 @@
     </row>
     <row r="74" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="H74" s="1">
         <v>2011</v>
@@ -4222,21 +4222,21 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="H75" s="1">
         <v>2011</v>
@@ -4244,21 +4244,21 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="H76" s="1">
         <v>2012</v>
@@ -4266,21 +4266,21 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>284</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="H77" s="1">
         <v>2003</v>
@@ -4288,18 +4288,18 @@
     </row>
     <row r="78" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1">
@@ -4308,21 +4308,21 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="H79" s="1">
         <v>2010</v>
@@ -4330,21 +4330,21 @@
     </row>
     <row r="80" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="H80" s="1">
         <v>1998</v>
@@ -4352,21 +4352,21 @@
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H81" s="1">
         <v>2003</v>
@@ -4374,21 +4374,21 @@
     </row>
     <row r="82" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H82" s="1">
         <v>1998</v>
@@ -4396,21 +4396,21 @@
     </row>
     <row r="83" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="H83" s="1">
         <v>2010</v>
@@ -4418,21 +4418,21 @@
     </row>
     <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H84" s="1">
         <v>2007</v>
@@ -4440,21 +4440,21 @@
     </row>
     <row r="85" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H85" s="1">
         <v>2008</v>
@@ -4462,21 +4462,21 @@
     </row>
     <row r="86" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>306</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="H86" s="1">
         <v>1997</v>
@@ -4484,21 +4484,21 @@
     </row>
     <row r="87" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="H87" s="1">
         <v>2005</v>
@@ -4506,21 +4506,21 @@
     </row>
     <row r="88" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="H88" s="1">
         <v>2010</v>
@@ -4528,21 +4528,21 @@
     </row>
     <row r="89" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G89" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="H89" s="1">
         <v>2007</v>
@@ -4550,18 +4550,18 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1">
@@ -4570,21 +4570,21 @@
     </row>
     <row r="91" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>325</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="H91" s="1">
         <v>2012</v>
@@ -4592,19 +4592,19 @@
     </row>
     <row r="92" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G92" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="H92" s="1">
         <v>2013</v>
@@ -4612,18 +4612,18 @@
     </row>
     <row r="93" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G93" s="1"/>
       <c r="H93" s="1">
@@ -4632,19 +4632,19 @@
     </row>
     <row r="94" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G94" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>337</v>
       </c>
       <c r="H94" s="1">
         <v>2005</v>
@@ -4652,21 +4652,21 @@
     </row>
     <row r="95" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="H95" s="1">
         <v>1998</v>
@@ -4674,21 +4674,21 @@
     </row>
     <row r="96" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="G96" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="H96" s="1">
         <v>2008</v>
@@ -4696,21 +4696,21 @@
     </row>
     <row r="97" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="G97" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="H97" s="1">
         <v>2006</v>
@@ -4718,16 +4718,16 @@
     </row>
     <row r="98" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="1">
@@ -4736,21 +4736,21 @@
     </row>
     <row r="99" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>354</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="H99" s="1">
         <v>2008</v>
@@ -4758,16 +4758,16 @@
     </row>
     <row r="100" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" s="1">
@@ -4776,21 +4776,21 @@
     </row>
     <row r="101" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>362</v>
       </c>
       <c r="H101" s="1">
         <v>2010</v>
@@ -4798,18 +4798,18 @@
     </row>
     <row r="102" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>364</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="1">
@@ -4818,21 +4818,21 @@
     </row>
     <row r="103" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>370</v>
       </c>
       <c r="H103" s="1">
         <v>2010</v>
@@ -4840,49 +4840,49 @@
     </row>
     <row r="104" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G104" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="H104" s="1"/>
     </row>
     <row r="105" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H105" s="1"/>
     </row>
     <row r="106" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G106" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="H106" s="1">
         <v>2004</v>
@@ -4890,17 +4890,17 @@
     </row>
     <row r="107" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>378</v>
       </c>
       <c r="H107" s="1">
         <v>1966</v>
@@ -4908,18 +4908,18 @@
     </row>
     <row r="108" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>380</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>381</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G108" s="1"/>
       <c r="H108" s="1">
@@ -4928,21 +4928,21 @@
     </row>
     <row r="109" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>384</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="H109" s="1">
         <v>2007</v>
@@ -4950,21 +4950,21 @@
     </row>
     <row r="110" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G110" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="H110" s="1">
         <v>2005</v>
@@ -4972,21 +4972,21 @@
     </row>
     <row r="111" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>392</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>394</v>
       </c>
       <c r="H111" s="1">
         <v>2003</v>
@@ -4994,21 +4994,21 @@
     </row>
     <row r="112" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>396</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G112" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>398</v>
       </c>
       <c r="H112" s="1">
         <v>2010</v>
@@ -5016,21 +5016,21 @@
     </row>
     <row r="113" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>400</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>402</v>
       </c>
       <c r="H113" s="1">
         <v>2007</v>
@@ -5038,21 +5038,21 @@
     </row>
     <row r="114" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G114" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>406</v>
       </c>
       <c r="H114" s="1">
         <v>2012</v>
@@ -5060,21 +5060,21 @@
     </row>
     <row r="115" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>410</v>
       </c>
       <c r="H115" s="1">
         <v>2003</v>
@@ -5082,21 +5082,21 @@
     </row>
     <row r="116" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>412</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G116" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>414</v>
       </c>
       <c r="H116" s="1">
         <v>2002</v>
@@ -5104,21 +5104,21 @@
     </row>
     <row r="117" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="H117" s="1">
         <v>1998</v>
@@ -5126,19 +5126,19 @@
     </row>
     <row r="118" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G118" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>421</v>
       </c>
       <c r="H118" s="1">
         <v>2002</v>
@@ -5146,21 +5146,21 @@
     </row>
     <row r="119" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>423</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G119" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>425</v>
       </c>
       <c r="H119" s="1">
         <v>2005</v>
@@ -5168,21 +5168,21 @@
     </row>
     <row r="120" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>427</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G120" s="1" t="s">
         <v>428</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>429</v>
       </c>
       <c r="H120" s="1">
         <v>2013</v>
@@ -5190,21 +5190,21 @@
     </row>
     <row r="121" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>431</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>433</v>
       </c>
       <c r="H121" s="1">
         <v>2011</v>
@@ -5212,21 +5212,21 @@
     </row>
     <row r="122" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>435</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>437</v>
       </c>
       <c r="H122" s="1">
         <v>2008</v>
@@ -5234,18 +5234,18 @@
     </row>
     <row r="123" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>439</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="1">
@@ -5254,21 +5254,21 @@
     </row>
     <row r="124" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>439</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G124" s="1" t="s">
         <v>441</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>442</v>
       </c>
       <c r="H124" s="1">
         <v>2014</v>
@@ -5276,18 +5276,18 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>444</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G125" s="1"/>
       <c r="H125" s="1">
@@ -5296,21 +5296,21 @@
     </row>
     <row r="126" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>447</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G126" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="H126" s="1">
         <v>2010</v>
@@ -5318,18 +5318,18 @@
     </row>
     <row r="127" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" s="1">
@@ -5338,18 +5338,18 @@
     </row>
     <row r="128" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>453</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="1">
@@ -5358,21 +5358,21 @@
     </row>
     <row r="129" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>456</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G129" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>458</v>
       </c>
       <c r="H129" s="1">
         <v>2006</v>
@@ -5380,21 +5380,21 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="G130" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="H130" s="1">
         <v>2012</v>
@@ -5402,21 +5402,21 @@
     </row>
     <row r="131" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>464</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G131" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="G131" s="1" t="s">
-        <v>466</v>
       </c>
       <c r="H131" s="1">
         <v>2012</v>
@@ -5424,21 +5424,21 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>468</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H132" s="1">
         <v>2013</v>
@@ -5446,19 +5446,19 @@
     </row>
     <row r="133" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>472</v>
       </c>
       <c r="H133" s="1">
         <v>2001</v>
@@ -5466,18 +5466,18 @@
     </row>
     <row r="134" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G134" s="1"/>
       <c r="H134" s="1">
@@ -5486,18 +5486,18 @@
     </row>
     <row r="135" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D135" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>476</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G135" s="1"/>
       <c r="H135" s="1">
@@ -5506,21 +5506,21 @@
     </row>
     <row r="136" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D136" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>479</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G136" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>481</v>
       </c>
       <c r="H136" s="1">
         <v>2007</v>
@@ -5528,16 +5528,16 @@
     </row>
     <row r="137" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" s="1">
@@ -5546,21 +5546,21 @@
     </row>
     <row r="138" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>484</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>485</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="G138" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>487</v>
       </c>
       <c r="H138" s="1">
         <v>1978</v>
@@ -5568,21 +5568,21 @@
     </row>
     <row r="139" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>489</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="G139" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>491</v>
       </c>
       <c r="H139" s="1">
         <v>1992</v>
@@ -5590,21 +5590,21 @@
     </row>
     <row r="140" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="G140" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>495</v>
       </c>
       <c r="H140" s="1">
         <v>2000</v>
@@ -5612,20 +5612,20 @@
     </row>
     <row r="141" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D141" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="E141" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F141" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="G141" s="1"/>
       <c r="H141" s="1">
@@ -5634,21 +5634,21 @@
     </row>
     <row r="142" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D142" s="1" t="s">
         <v>499</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>500</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="G142" s="1" t="s">
         <v>501</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>502</v>
       </c>
       <c r="H142" s="1">
         <v>2009</v>
@@ -5656,21 +5656,21 @@
     </row>
     <row r="143" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>504</v>
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="G143" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>506</v>
       </c>
       <c r="H143" s="1">
         <v>2011</v>
@@ -5678,20 +5678,20 @@
     </row>
     <row r="144" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="E144" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F144" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>509</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="1">
@@ -5700,21 +5700,21 @@
     </row>
     <row r="145" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D145" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>512</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="G145" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>514</v>
       </c>
       <c r="H145" s="1">
         <v>2013</v>
@@ -5722,21 +5722,21 @@
     </row>
     <row r="146" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H146" s="1">
         <v>2010</v>
@@ -5744,21 +5744,21 @@
     </row>
     <row r="147" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D147" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>519</v>
       </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="G147" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>521</v>
       </c>
       <c r="H147" s="1">
         <v>2005</v>
@@ -5766,18 +5766,18 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D148" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>523</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G148" s="1"/>
       <c r="H148" s="1">
@@ -5786,21 +5786,21 @@
     </row>
     <row r="149" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>526</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H149" s="1">
         <v>2011</v>
@@ -5808,18 +5808,18 @@
     </row>
     <row r="150" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D150" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>529</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G150" s="1"/>
       <c r="H150" s="1">
@@ -5828,20 +5828,20 @@
     </row>
     <row r="151" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D151" s="1" t="s">
+      <c r="E151" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F151" s="1" t="s">
         <v>532</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>533</v>
       </c>
       <c r="G151" s="1"/>
       <c r="H151" s="1">
@@ -5850,21 +5850,21 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>535</v>
       </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="G152" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>537</v>
       </c>
       <c r="H152" s="1">
         <v>2004</v>
@@ -5872,21 +5872,21 @@
     </row>
     <row r="153" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>540</v>
       </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="G153" s="1" t="s">
         <v>541</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>542</v>
       </c>
       <c r="H153" s="1">
         <v>2010</v>
@@ -5894,21 +5894,21 @@
     </row>
     <row r="154" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>544</v>
       </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H154" s="1">
         <v>2012</v>
@@ -5916,18 +5916,18 @@
     </row>
     <row r="155" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>548</v>
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G155" s="1"/>
       <c r="H155" s="1">

</xml_diff>

<commit_message>
updated with edm and muk versions
</commit_message>
<xml_diff>
--- a/Macro File/daily rtf test.xlsx
+++ b/Macro File/daily rtf test.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Daily RTF report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -143,9 +143,6 @@
     <t>Compact Disc</t>
   </si>
   <si>
-    <t>CD M RHYE</t>
-  </si>
-  <si>
     <t>Rhye (Musical group)</t>
   </si>
   <si>
@@ -1673,7 +1670,10 @@
     <t>Debunk it! : how to stay sane in a world of misinformation</t>
   </si>
   <si>
-    <t>CD MRI BUCKCHE</t>
+    <t>CD MR BUCKCHE</t>
+  </si>
+  <si>
+    <t>CD MR RHYE</t>
   </si>
 </sst>
 </file>
@@ -2017,7 +2017,7 @@
   <dimension ref="A1:H156"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2850,17 +2850,17 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="H9" s="1">
         <v>2012</v>
@@ -2872,17 +2872,17 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="H10" s="1">
         <v>2003</v>
@@ -2894,17 +2894,17 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="H11" s="1">
         <v>2009</v>
@@ -2916,17 +2916,17 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="H12" s="1">
         <v>2011</v>
@@ -2938,17 +2938,17 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H13" s="1">
         <v>2011</v>
@@ -2960,17 +2960,17 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="H14" s="1">
         <v>2012</v>
@@ -2982,17 +2982,17 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="H15" s="1">
         <v>2011</v>
@@ -3004,17 +3004,17 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H16" s="1">
         <v>2009</v>
@@ -3026,17 +3026,17 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="H17" s="1">
         <v>1993</v>
@@ -3044,19 +3044,19 @@
     </row>
     <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="H18" s="1">
         <v>2010</v>
@@ -3064,19 +3064,19 @@
     </row>
     <row r="19" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="H19" s="1">
         <v>2000</v>
@@ -3084,19 +3084,19 @@
     </row>
     <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="H20" s="1">
         <v>2009</v>
@@ -3104,19 +3104,19 @@
     </row>
     <row r="21" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="H21" s="1">
         <v>2011</v>
@@ -3124,19 +3124,19 @@
     </row>
     <row r="22" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="H22" s="1">
         <v>2007</v>
@@ -3144,16 +3144,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1">
@@ -3162,19 +3162,19 @@
     </row>
     <row r="24" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="H24" s="1">
         <v>1998</v>
@@ -3182,19 +3182,19 @@
     </row>
     <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="H25" s="1">
         <v>1995</v>
@@ -3202,19 +3202,19 @@
     </row>
     <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="H26" s="1">
         <v>2013</v>
@@ -3222,16 +3222,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1">
@@ -3240,19 +3240,19 @@
     </row>
     <row r="28" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="H28" s="1">
         <v>2007</v>
@@ -3260,19 +3260,19 @@
     </row>
     <row r="29" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H29" s="1">
         <v>2012</v>
@@ -3280,19 +3280,19 @@
     </row>
     <row r="30" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="H30" s="1">
         <v>2006</v>
@@ -3300,19 +3300,19 @@
     </row>
     <row r="31" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H31" s="1">
         <v>2008</v>
@@ -3320,16 +3320,16 @@
     </row>
     <row r="32" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1">
@@ -3338,19 +3338,19 @@
     </row>
     <row r="33" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="H33" s="1">
         <v>2009</v>
@@ -3358,19 +3358,19 @@
     </row>
     <row r="34" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H34" s="1">
         <v>2004</v>
@@ -3378,19 +3378,19 @@
     </row>
     <row r="35" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="H35" s="1">
         <v>1999</v>
@@ -3398,19 +3398,19 @@
     </row>
     <row r="36" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="H36" s="1">
         <v>2003</v>
@@ -3418,19 +3418,19 @@
     </row>
     <row r="37" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H37" s="1">
         <v>2010</v>
@@ -3438,19 +3438,19 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="H38" s="1">
         <v>2014</v>
@@ -3458,19 +3458,19 @@
     </row>
     <row r="39" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="H39" s="1">
         <v>2006</v>
@@ -3478,19 +3478,19 @@
     </row>
     <row r="40" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="H40" s="1">
         <v>2011</v>
@@ -3498,16 +3498,16 @@
     </row>
     <row r="41" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1">
@@ -3516,16 +3516,16 @@
     </row>
     <row r="42" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1">
@@ -3534,19 +3534,19 @@
     </row>
     <row r="43" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="H43" s="1">
         <v>2006</v>
@@ -3554,19 +3554,19 @@
     </row>
     <row r="44" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H44" s="1">
         <v>2008</v>
@@ -3574,21 +3574,21 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="H45" s="1">
         <v>1978</v>
@@ -3596,21 +3596,21 @@
     </row>
     <row r="46" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="H46" s="1">
         <v>2014</v>
@@ -3618,18 +3618,18 @@
     </row>
     <row r="47" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1">
@@ -3638,21 +3638,21 @@
     </row>
     <row r="48" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="H48" s="1">
         <v>2010</v>
@@ -3660,21 +3660,21 @@
     </row>
     <row r="49" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="H49" s="1">
         <v>2008</v>
@@ -3682,21 +3682,21 @@
     </row>
     <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="H50" s="1">
         <v>2012</v>
@@ -3704,21 +3704,21 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="H51" s="1">
         <v>2008</v>
@@ -3726,21 +3726,21 @@
     </row>
     <row r="52" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="H52" s="1">
         <v>1991</v>
@@ -3748,21 +3748,21 @@
     </row>
     <row r="53" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="H53" s="1">
         <v>2003</v>
@@ -3770,21 +3770,21 @@
     </row>
     <row r="54" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H54" s="1">
         <v>1987</v>
@@ -3792,21 +3792,21 @@
     </row>
     <row r="55" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="H55" s="1">
         <v>2008</v>
@@ -3814,21 +3814,21 @@
     </row>
     <row r="56" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="H56" s="1">
         <v>2002</v>
@@ -3836,19 +3836,19 @@
     </row>
     <row r="57" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="H57" s="1">
         <v>1973</v>
@@ -3856,21 +3856,21 @@
     </row>
     <row r="58" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="H58" s="1">
         <v>2011</v>
@@ -3878,21 +3878,21 @@
     </row>
     <row r="59" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="H59" s="1">
         <v>2004</v>
@@ -3900,23 +3900,23 @@
     </row>
     <row r="60" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="H60" s="1">
         <v>2003</v>
@@ -3924,21 +3924,21 @@
     </row>
     <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="H61" s="1">
         <v>2011</v>
@@ -3946,21 +3946,21 @@
     </row>
     <row r="62" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="H62" s="1">
         <v>2014</v>
@@ -3968,20 +3968,20 @@
     </row>
     <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1">
@@ -3990,18 +3990,18 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1">
@@ -4010,18 +4010,18 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1">
@@ -4030,18 +4030,18 @@
     </row>
     <row r="66" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1">
@@ -4050,20 +4050,20 @@
     </row>
     <row r="67" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1">
@@ -4072,21 +4072,21 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="H68" s="1">
         <v>2012</v>
@@ -4094,18 +4094,18 @@
     </row>
     <row r="69" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1">
@@ -4114,18 +4114,18 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="1">
@@ -4134,21 +4134,21 @@
     </row>
     <row r="71" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="H71" s="1">
         <v>2006</v>
@@ -4156,21 +4156,21 @@
     </row>
     <row r="72" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="H72" s="1">
         <v>2014</v>
@@ -4178,21 +4178,21 @@
     </row>
     <row r="73" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H73" s="1">
         <v>1996</v>
@@ -4200,21 +4200,21 @@
     </row>
     <row r="74" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="H74" s="1">
         <v>2011</v>
@@ -4222,21 +4222,21 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="H75" s="1">
         <v>2011</v>
@@ -4244,21 +4244,21 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="H76" s="1">
         <v>2012</v>
@@ -4266,21 +4266,21 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="H77" s="1">
         <v>2003</v>
@@ -4288,18 +4288,18 @@
     </row>
     <row r="78" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G78" s="1"/>
       <c r="H78" s="1">
@@ -4308,21 +4308,21 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="H79" s="1">
         <v>2010</v>
@@ -4330,21 +4330,21 @@
     </row>
     <row r="80" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="H80" s="1">
         <v>1998</v>
@@ -4352,21 +4352,21 @@
     </row>
     <row r="81" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H81" s="1">
         <v>2003</v>
@@ -4374,21 +4374,21 @@
     </row>
     <row r="82" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H82" s="1">
         <v>1998</v>
@@ -4396,21 +4396,21 @@
     </row>
     <row r="83" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="H83" s="1">
         <v>2010</v>
@@ -4418,21 +4418,21 @@
     </row>
     <row r="84" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H84" s="1">
         <v>2007</v>
@@ -4440,21 +4440,21 @@
     </row>
     <row r="85" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H85" s="1">
         <v>2008</v>
@@ -4462,21 +4462,21 @@
     </row>
     <row r="86" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="H86" s="1">
         <v>1997</v>
@@ -4484,21 +4484,21 @@
     </row>
     <row r="87" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>309</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="H87" s="1">
         <v>2005</v>
@@ -4506,21 +4506,21 @@
     </row>
     <row r="88" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G88" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="H88" s="1">
         <v>2010</v>
@@ -4528,21 +4528,21 @@
     </row>
     <row r="89" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G89" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="H89" s="1">
         <v>2007</v>
@@ -4550,18 +4550,18 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="1">
@@ -4570,21 +4570,21 @@
     </row>
     <row r="91" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="H91" s="1">
         <v>2012</v>
@@ -4592,19 +4592,19 @@
     </row>
     <row r="92" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G92" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>330</v>
       </c>
       <c r="H92" s="1">
         <v>2013</v>
@@ -4612,18 +4612,18 @@
     </row>
     <row r="93" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G93" s="1"/>
       <c r="H93" s="1">
@@ -4632,19 +4632,19 @@
     </row>
     <row r="94" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G94" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="H94" s="1">
         <v>2005</v>
@@ -4652,21 +4652,21 @@
     </row>
     <row r="95" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>341</v>
       </c>
       <c r="H95" s="1">
         <v>1998</v>
@@ -4674,21 +4674,21 @@
     </row>
     <row r="96" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G96" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="H96" s="1">
         <v>2008</v>
@@ -4696,21 +4696,21 @@
     </row>
     <row r="97" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="G97" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="H97" s="1">
         <v>2006</v>
@@ -4718,16 +4718,16 @@
     </row>
     <row r="98" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="1">
@@ -4736,21 +4736,21 @@
     </row>
     <row r="99" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="H99" s="1">
         <v>2008</v>
@@ -4758,16 +4758,16 @@
     </row>
     <row r="100" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" s="1">
@@ -4776,21 +4776,21 @@
     </row>
     <row r="101" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D101" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>359</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="H101" s="1">
         <v>2010</v>
@@ -4798,18 +4798,18 @@
     </row>
     <row r="102" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="1">
@@ -4818,21 +4818,21 @@
     </row>
     <row r="103" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>367</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="H103" s="1">
         <v>2010</v>
@@ -4840,49 +4840,49 @@
     </row>
     <row r="104" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G104" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>372</v>
       </c>
       <c r="H104" s="1"/>
     </row>
     <row r="105" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H105" s="1"/>
     </row>
     <row r="106" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G106" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="H106" s="1">
         <v>2004</v>
@@ -4890,17 +4890,17 @@
     </row>
     <row r="107" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="H107" s="1">
         <v>1966</v>
@@ -4908,18 +4908,18 @@
     </row>
     <row r="108" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>380</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G108" s="1"/>
       <c r="H108" s="1">
@@ -4928,21 +4928,21 @@
     </row>
     <row r="109" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="H109" s="1">
         <v>2007</v>
@@ -4950,21 +4950,21 @@
     </row>
     <row r="110" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D110" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G110" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="H110" s="1">
         <v>2005</v>
@@ -4972,21 +4972,21 @@
     </row>
     <row r="111" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>393</v>
       </c>
       <c r="H111" s="1">
         <v>2003</v>
@@ -4994,21 +4994,21 @@
     </row>
     <row r="112" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>395</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G112" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>397</v>
       </c>
       <c r="H112" s="1">
         <v>2010</v>
@@ -5016,21 +5016,21 @@
     </row>
     <row r="113" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>399</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>401</v>
       </c>
       <c r="H113" s="1">
         <v>2007</v>
@@ -5038,21 +5038,21 @@
     </row>
     <row r="114" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>403</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G114" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>405</v>
       </c>
       <c r="H114" s="1">
         <v>2012</v>
@@ -5060,21 +5060,21 @@
     </row>
     <row r="115" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>407</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>409</v>
       </c>
       <c r="H115" s="1">
         <v>2003</v>
@@ -5082,21 +5082,21 @@
     </row>
     <row r="116" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>411</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="G116" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>413</v>
       </c>
       <c r="H116" s="1">
         <v>2002</v>
@@ -5104,21 +5104,21 @@
     </row>
     <row r="117" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>415</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>417</v>
       </c>
       <c r="H117" s="1">
         <v>1998</v>
@@ -5126,19 +5126,19 @@
     </row>
     <row r="118" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G118" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="H118" s="1">
         <v>2002</v>
@@ -5146,21 +5146,21 @@
     </row>
     <row r="119" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G119" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>424</v>
       </c>
       <c r="H119" s="1">
         <v>2005</v>
@@ -5168,21 +5168,21 @@
     </row>
     <row r="120" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G120" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="H120" s="1">
         <v>2013</v>
@@ -5190,21 +5190,21 @@
     </row>
     <row r="121" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="G121" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="H121" s="1">
         <v>2011</v>
@@ -5212,21 +5212,21 @@
     </row>
     <row r="122" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>434</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="H122" s="1">
         <v>2008</v>
@@ -5234,18 +5234,18 @@
     </row>
     <row r="123" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="1">
@@ -5254,21 +5254,21 @@
     </row>
     <row r="124" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="G124" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="G124" s="1" t="s">
-        <v>441</v>
       </c>
       <c r="H124" s="1">
         <v>2014</v>
@@ -5276,18 +5276,18 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>442</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>443</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G125" s="1"/>
       <c r="H125" s="1">
@@ -5296,21 +5296,21 @@
     </row>
     <row r="126" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G126" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>448</v>
       </c>
       <c r="H126" s="1">
         <v>2010</v>
@@ -5318,18 +5318,18 @@
     </row>
     <row r="127" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" s="1">
@@ -5338,18 +5338,18 @@
     </row>
     <row r="128" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>451</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>452</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="1">
@@ -5358,21 +5358,21 @@
     </row>
     <row r="129" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>455</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="G129" s="1" t="s">
         <v>456</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>457</v>
       </c>
       <c r="H129" s="1">
         <v>2006</v>
@@ -5380,21 +5380,21 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="G130" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="G130" s="1" t="s">
-        <v>461</v>
       </c>
       <c r="H130" s="1">
         <v>2012</v>
@@ -5402,21 +5402,21 @@
     </row>
     <row r="131" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>463</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G131" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="G131" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="H131" s="1">
         <v>2012</v>
@@ -5424,21 +5424,21 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>467</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H132" s="1">
         <v>2013</v>
@@ -5446,19 +5446,19 @@
     </row>
     <row r="133" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H133" s="1">
         <v>2001</v>
@@ -5466,18 +5466,18 @@
     </row>
     <row r="134" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G134" s="1"/>
       <c r="H134" s="1">
@@ -5486,18 +5486,18 @@
     </row>
     <row r="135" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D135" s="1" t="s">
         <v>474</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>475</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G135" s="1"/>
       <c r="H135" s="1">
@@ -5506,21 +5506,21 @@
     </row>
     <row r="136" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D136" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>478</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="G136" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>480</v>
       </c>
       <c r="H136" s="1">
         <v>2007</v>
@@ -5528,16 +5528,16 @@
     </row>
     <row r="137" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G137" s="1"/>
       <c r="H137" s="1">
@@ -5546,21 +5546,21 @@
     </row>
     <row r="138" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D138" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>484</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="G138" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="H138" s="1">
         <v>1978</v>
@@ -5568,21 +5568,21 @@
     </row>
     <row r="139" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>488</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="G139" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="G139" s="1" t="s">
-        <v>490</v>
       </c>
       <c r="H139" s="1">
         <v>1992</v>
@@ -5590,21 +5590,21 @@
     </row>
     <row r="140" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>492</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="G140" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>494</v>
       </c>
       <c r="H140" s="1">
         <v>2000</v>
@@ -5612,20 +5612,20 @@
     </row>
     <row r="141" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D141" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="E141" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F141" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>497</v>
       </c>
       <c r="G141" s="1"/>
       <c r="H141" s="1">
@@ -5634,21 +5634,21 @@
     </row>
     <row r="142" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D142" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="G142" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="G142" s="1" t="s">
-        <v>501</v>
       </c>
       <c r="H142" s="1">
         <v>2009</v>
@@ -5656,21 +5656,21 @@
     </row>
     <row r="143" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>503</v>
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G143" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>505</v>
       </c>
       <c r="H143" s="1">
         <v>2011</v>
@@ -5678,20 +5678,20 @@
     </row>
     <row r="144" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="E144" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F144" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>508</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="1">
@@ -5700,21 +5700,21 @@
     </row>
     <row r="145" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D145" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>511</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="G145" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>513</v>
       </c>
       <c r="H145" s="1">
         <v>2013</v>
@@ -5722,21 +5722,21 @@
     </row>
     <row r="146" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H146" s="1">
         <v>2010</v>
@@ -5744,21 +5744,21 @@
     </row>
     <row r="147" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D147" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="G147" s="1" t="s">
         <v>519</v>
-      </c>
-      <c r="G147" s="1" t="s">
-        <v>520</v>
       </c>
       <c r="H147" s="1">
         <v>2005</v>
@@ -5766,18 +5766,18 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D148" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>522</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G148" s="1"/>
       <c r="H148" s="1">
@@ -5786,21 +5786,21 @@
     </row>
     <row r="149" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>525</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H149" s="1">
         <v>2011</v>
@@ -5808,18 +5808,18 @@
     </row>
     <row r="150" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D150" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>528</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G150" s="1"/>
       <c r="H150" s="1">
@@ -5828,20 +5828,20 @@
     </row>
     <row r="151" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="D151" s="1" t="s">
+      <c r="E151" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F151" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>532</v>
       </c>
       <c r="G151" s="1"/>
       <c r="H151" s="1">
@@ -5850,21 +5850,21 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D152" s="1" t="s">
         <v>533</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>534</v>
       </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G152" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>536</v>
       </c>
       <c r="H152" s="1">
         <v>2004</v>
@@ -5872,21 +5872,21 @@
     </row>
     <row r="153" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>539</v>
       </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="G153" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="G153" s="1" t="s">
-        <v>541</v>
       </c>
       <c r="H153" s="1">
         <v>2010</v>
@@ -5894,21 +5894,21 @@
     </row>
     <row r="154" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>543</v>
       </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H154" s="1">
         <v>2012</v>
@@ -5916,18 +5916,18 @@
     </row>
     <row r="155" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>547</v>
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G155" s="1"/>
       <c r="H155" s="1">

</xml_diff>